<commit_message>
[MS-COPYS] Add and update cases and capture code for latest RS
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="701">
   <si>
     <t>Req ID</t>
   </si>
@@ -2506,14 +2506,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2709,13 +2709,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2748,7 +2748,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2771,6 +2771,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2794,21 +2809,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3757,127 +3757,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -3890,12 +3890,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -3908,12 +3908,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -3926,12 +3926,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -3944,60 +3944,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="45">
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="30" t="s">
         <v>65</v>
       </c>
@@ -4658,7 +4658,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="180">
+    <row r="45" spans="1:9" ht="165">
       <c r="A45" s="22" t="s">
         <v>68</v>
       </c>
@@ -5083,7 +5083,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="90">
+    <row r="62" spans="1:9" ht="75">
       <c r="A62" s="30" t="s">
         <v>85</v>
       </c>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="45">
+    <row r="69" spans="1:9" ht="30">
       <c r="A69" s="30" t="s">
         <v>92</v>
       </c>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="45">
+    <row r="70" spans="1:9" ht="30">
       <c r="A70" s="30" t="s">
         <v>93</v>
       </c>
@@ -5849,7 +5849,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="105">
+    <row r="92" spans="1:9" ht="90">
       <c r="A92" s="30" t="s">
         <v>115</v>
       </c>
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9" ht="30">
+    <row r="93" spans="1:9">
       <c r="A93" s="30" t="s">
         <v>116</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="60">
+    <row r="126" spans="1:9" ht="45">
       <c r="A126" s="30" t="s">
         <v>147</v>
       </c>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" ht="45" hidden="1">
+    <row r="134" spans="1:9" ht="30" hidden="1">
       <c r="A134" s="30" t="s">
         <v>155</v>
       </c>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9">
       <c r="A164" s="30" t="s">
         <v>185</v>
       </c>
@@ -8516,7 +8516,7 @@
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9" ht="30">
+    <row r="197" spans="1:9">
       <c r="A197" s="30" t="s">
         <v>217</v>
       </c>
@@ -8591,7 +8591,7 @@
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="45">
+    <row r="200" spans="1:9" ht="30">
       <c r="A200" s="30" t="s">
         <v>220</v>
       </c>
@@ -9066,7 +9066,7 @@
       </c>
       <c r="I218" s="32"/>
     </row>
-    <row r="219" spans="1:9" ht="60">
+    <row r="219" spans="1:9" ht="45">
       <c r="A219" s="22" t="s">
         <v>239</v>
       </c>
@@ -9318,7 +9318,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9" ht="30">
+    <row r="229" spans="1:9">
       <c r="A229" s="30" t="s">
         <v>249</v>
       </c>
@@ -9368,7 +9368,7 @@
       </c>
       <c r="I230" s="32"/>
     </row>
-    <row r="231" spans="1:9" ht="180">
+    <row r="231" spans="1:9" ht="165">
       <c r="A231" s="30" t="s">
         <v>251</v>
       </c>
@@ -10068,7 +10068,7 @@
       </c>
       <c r="I258" s="32"/>
     </row>
-    <row r="259" spans="1:9" ht="60">
+    <row r="259" spans="1:9" ht="45">
       <c r="A259" s="22" t="s">
         <v>279</v>
       </c>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="I272" s="32"/>
     </row>
-    <row r="273" spans="1:9" ht="60">
+    <row r="273" spans="1:9" ht="45">
       <c r="A273" s="30" t="s">
         <v>293</v>
       </c>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="I279" s="32"/>
     </row>
-    <row r="280" spans="1:9" ht="150">
+    <row r="280" spans="1:9" ht="135">
       <c r="A280" s="30" t="s">
         <v>300</v>
       </c>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="I287" s="32"/>
     </row>
-    <row r="288" spans="1:9" ht="30">
+    <row r="288" spans="1:9">
       <c r="A288" s="30" t="s">
         <v>308</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="301" spans="1:9" ht="45">
+    <row r="301" spans="1:9" ht="30">
       <c r="A301" s="22" t="s">
         <v>666</v>
       </c>
@@ -11189,13 +11189,11 @@
         <v>15</v>
       </c>
       <c r="H301" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I301" s="32" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="302" spans="1:9" ht="45">
+        <v>18</v>
+      </c>
+      <c r="I301" s="32"/>
+    </row>
+    <row r="302" spans="1:9" ht="30">
       <c r="A302" s="22" t="s">
         <v>671</v>
       </c>
@@ -11218,11 +11216,9 @@
         <v>15</v>
       </c>
       <c r="H302" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I302" s="32" t="s">
-        <v>651</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I302" s="32"/>
     </row>
     <row r="303" spans="1:9" ht="45">
       <c r="A303" s="30" t="s">
@@ -11305,11 +11301,9 @@
         <v>15</v>
       </c>
       <c r="H305" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I305" s="32" t="s">
-        <v>651</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I305" s="32"/>
     </row>
     <row r="306" spans="1:9" ht="45">
       <c r="A306" s="22" t="s">
@@ -11429,11 +11423,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -11441,6 +11430,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I309">
@@ -11507,21 +11501,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -11570,10 +11549,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11593,16 +11594,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-COPYS]: Fix watchman warnings.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -2492,8 +2492,7 @@
     <t>MS-COPYS_R280:i</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-COPYS_R12332.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Verified by derived requirement: MS-COPYS_R12332.</t>
   </si>
 </sst>
 </file>
@@ -2501,14 +2500,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2704,13 +2703,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2743,7 +2742,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3322,13 +3321,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I309" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I309">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Normative"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A19:I309"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -4178,7 +4171,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" hidden="1">
+    <row r="26" spans="1:12" s="23" customFormat="1">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -4203,7 +4196,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -4228,7 +4221,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -4253,7 +4246,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="45" hidden="1">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
@@ -4278,7 +4271,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" hidden="1">
+    <row r="30" spans="1:12" s="23" customFormat="1">
       <c r="A30" s="22" t="s">
         <v>53</v>
       </c>
@@ -4303,7 +4296,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" hidden="1">
+    <row r="31" spans="1:12" s="23" customFormat="1">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -4328,7 +4321,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" hidden="1">
+    <row r="32" spans="1:12" s="23" customFormat="1">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -4353,7 +4346,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" hidden="1">
+    <row r="33" spans="1:9" s="23" customFormat="1">
       <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
@@ -4378,7 +4371,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9">
       <c r="A34" s="30" t="s">
         <v>57</v>
       </c>
@@ -4403,7 +4396,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9">
       <c r="A35" s="30" t="s">
         <v>58</v>
       </c>
@@ -4428,7 +4421,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" hidden="1">
+    <row r="36" spans="1:9">
       <c r="A36" s="30" t="s">
         <v>59</v>
       </c>
@@ -4453,7 +4446,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30" hidden="1">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="30" t="s">
         <v>60</v>
       </c>
@@ -4503,7 +4496,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30" hidden="1">
+    <row r="39" spans="1:9" ht="30">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>
@@ -4553,7 +4546,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
         <v>64</v>
       </c>
@@ -4578,7 +4571,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9" ht="45">
       <c r="A42" s="30" t="s">
         <v>65</v>
       </c>
@@ -4603,7 +4596,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="30" hidden="1">
+    <row r="43" spans="1:9" ht="30">
       <c r="A43" s="30" t="s">
         <v>66</v>
       </c>
@@ -4628,7 +4621,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30" hidden="1">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="30" t="s">
         <v>67</v>
       </c>
@@ -4653,7 +4646,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="165">
+    <row r="45" spans="1:9" ht="180">
       <c r="A45" s="22" t="s">
         <v>68</v>
       </c>
@@ -4678,7 +4671,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" hidden="1">
+    <row r="46" spans="1:9">
       <c r="A46" s="30" t="s">
         <v>69</v>
       </c>
@@ -4753,7 +4746,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9">
       <c r="A49" s="30" t="s">
         <v>72</v>
       </c>
@@ -4778,7 +4771,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="30" hidden="1">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="30" t="s">
         <v>73</v>
       </c>
@@ -4803,7 +4796,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30" hidden="1">
+    <row r="51" spans="1:9" ht="30">
       <c r="A51" s="30" t="s">
         <v>74</v>
       </c>
@@ -4828,7 +4821,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="30" hidden="1">
+    <row r="52" spans="1:9" ht="30">
       <c r="A52" s="30" t="s">
         <v>75</v>
       </c>
@@ -4853,7 +4846,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="30" hidden="1">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="30" t="s">
         <v>76</v>
       </c>
@@ -4878,7 +4871,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="30" hidden="1">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="30" t="s">
         <v>77</v>
       </c>
@@ -4903,7 +4896,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30" hidden="1">
+    <row r="55" spans="1:9" ht="30">
       <c r="A55" s="30" t="s">
         <v>78</v>
       </c>
@@ -4928,7 +4921,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30" hidden="1">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="30" t="s">
         <v>79</v>
       </c>
@@ -4953,7 +4946,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="30" hidden="1">
+    <row r="57" spans="1:9" ht="30">
       <c r="A57" s="30" t="s">
         <v>80</v>
       </c>
@@ -5003,7 +4996,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9">
       <c r="A59" s="30" t="s">
         <v>82</v>
       </c>
@@ -5053,7 +5046,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30" hidden="1">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="30" t="s">
         <v>84</v>
       </c>
@@ -5078,7 +5071,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="75">
+    <row r="62" spans="1:9" ht="90">
       <c r="A62" s="30" t="s">
         <v>85</v>
       </c>
@@ -5257,7 +5250,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9" ht="45">
       <c r="A69" s="30" t="s">
         <v>92</v>
       </c>
@@ -5284,7 +5277,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9" ht="45">
       <c r="A70" s="30" t="s">
         <v>93</v>
       </c>
@@ -5336,7 +5329,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="30" hidden="1">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="30" t="s">
         <v>95</v>
       </c>
@@ -5436,7 +5429,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30" hidden="1">
+    <row r="76" spans="1:9" ht="30">
       <c r="A76" s="30" t="s">
         <v>99</v>
       </c>
@@ -5461,7 +5454,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9">
       <c r="A77" s="30" t="s">
         <v>100</v>
       </c>
@@ -5511,7 +5504,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" s="30" t="s">
         <v>102</v>
       </c>
@@ -5711,7 +5704,7 @@
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="30" hidden="1">
+    <row r="87" spans="1:9" ht="30">
       <c r="A87" s="30" t="s">
         <v>110</v>
       </c>
@@ -5844,7 +5837,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="90">
+    <row r="92" spans="1:9" ht="105">
       <c r="A92" s="30" t="s">
         <v>115</v>
       </c>
@@ -5869,7 +5862,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" ht="30">
       <c r="A93" s="30" t="s">
         <v>116</v>
       </c>
@@ -5894,7 +5887,7 @@
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" ht="30" hidden="1">
+    <row r="94" spans="1:9" ht="30">
       <c r="A94" s="30" t="s">
         <v>117</v>
       </c>
@@ -5919,7 +5912,7 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="30" hidden="1">
+    <row r="95" spans="1:9" ht="30">
       <c r="A95" s="30" t="s">
         <v>118</v>
       </c>
@@ -5944,7 +5937,7 @@
       </c>
       <c r="I95" s="32"/>
     </row>
-    <row r="96" spans="1:9" ht="30" hidden="1">
+    <row r="96" spans="1:9" ht="30">
       <c r="A96" s="30" t="s">
         <v>119</v>
       </c>
@@ -5969,7 +5962,7 @@
       </c>
       <c r="I96" s="32"/>
     </row>
-    <row r="97" spans="1:9" ht="30" hidden="1">
+    <row r="97" spans="1:9" ht="30">
       <c r="A97" s="30" t="s">
         <v>120</v>
       </c>
@@ -5994,7 +5987,7 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30" hidden="1">
+    <row r="98" spans="1:9" ht="30">
       <c r="A98" s="30" t="s">
         <v>121</v>
       </c>
@@ -6019,7 +6012,7 @@
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="30" hidden="1">
+    <row r="99" spans="1:9" ht="30">
       <c r="A99" s="30" t="s">
         <v>122</v>
       </c>
@@ -6510,7 +6503,7 @@
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" hidden="1">
+    <row r="118" spans="1:9">
       <c r="A118" s="30" t="s">
         <v>141</v>
       </c>
@@ -6560,7 +6553,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="60" hidden="1">
+    <row r="120" spans="1:9" ht="60">
       <c r="A120" s="30" t="s">
         <v>143</v>
       </c>
@@ -6716,7 +6709,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="45">
+    <row r="126" spans="1:9" ht="60">
       <c r="A126" s="30" t="s">
         <v>147</v>
       </c>
@@ -6741,7 +6734,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" hidden="1">
+    <row r="127" spans="1:9">
       <c r="A127" s="30" t="s">
         <v>148</v>
       </c>
@@ -6791,7 +6784,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" hidden="1">
+    <row r="129" spans="1:9">
       <c r="A129" s="30" t="s">
         <v>150</v>
       </c>
@@ -6816,7 +6809,7 @@
       </c>
       <c r="I129" s="32"/>
     </row>
-    <row r="130" spans="1:9" hidden="1">
+    <row r="130" spans="1:9">
       <c r="A130" s="30" t="s">
         <v>151</v>
       </c>
@@ -6841,7 +6834,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" hidden="1">
+    <row r="131" spans="1:9">
       <c r="A131" s="30" t="s">
         <v>152</v>
       </c>
@@ -6866,7 +6859,7 @@
       </c>
       <c r="I131" s="32"/>
     </row>
-    <row r="132" spans="1:9" hidden="1">
+    <row r="132" spans="1:9">
       <c r="A132" s="30" t="s">
         <v>153</v>
       </c>
@@ -6891,7 +6884,7 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" hidden="1">
+    <row r="133" spans="1:9">
       <c r="A133" s="30" t="s">
         <v>154</v>
       </c>
@@ -6916,7 +6909,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" ht="30" hidden="1">
+    <row r="134" spans="1:9" ht="45">
       <c r="A134" s="30" t="s">
         <v>155</v>
       </c>
@@ -6941,7 +6934,7 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="30" hidden="1">
+    <row r="135" spans="1:9" ht="30">
       <c r="A135" s="30" t="s">
         <v>156</v>
       </c>
@@ -6966,7 +6959,7 @@
       </c>
       <c r="I135" s="32"/>
     </row>
-    <row r="136" spans="1:9" ht="30" hidden="1">
+    <row r="136" spans="1:9" ht="30">
       <c r="A136" s="30" t="s">
         <v>157</v>
       </c>
@@ -6991,7 +6984,7 @@
       </c>
       <c r="I136" s="32"/>
     </row>
-    <row r="137" spans="1:9" ht="30" hidden="1">
+    <row r="137" spans="1:9" ht="30">
       <c r="A137" s="30" t="s">
         <v>158</v>
       </c>
@@ -7016,7 +7009,7 @@
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="30" hidden="1">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="30" t="s">
         <v>159</v>
       </c>
@@ -7041,7 +7034,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" hidden="1">
+    <row r="139" spans="1:9">
       <c r="A139" s="30" t="s">
         <v>160</v>
       </c>
@@ -7066,7 +7059,7 @@
       </c>
       <c r="I139" s="32"/>
     </row>
-    <row r="140" spans="1:9" hidden="1">
+    <row r="140" spans="1:9">
       <c r="A140" s="30" t="s">
         <v>161</v>
       </c>
@@ -7091,7 +7084,7 @@
       </c>
       <c r="I140" s="32"/>
     </row>
-    <row r="141" spans="1:9" ht="30" hidden="1">
+    <row r="141" spans="1:9" ht="30">
       <c r="A141" s="30" t="s">
         <v>162</v>
       </c>
@@ -7116,7 +7109,7 @@
       </c>
       <c r="I141" s="32"/>
     </row>
-    <row r="142" spans="1:9" ht="30" hidden="1">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="30" t="s">
         <v>163</v>
       </c>
@@ -7218,7 +7211,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1">
+    <row r="146" spans="1:9">
       <c r="A146" s="30" t="s">
         <v>167</v>
       </c>
@@ -7268,7 +7261,7 @@
       </c>
       <c r="I147" s="32"/>
     </row>
-    <row r="148" spans="1:9" hidden="1">
+    <row r="148" spans="1:9">
       <c r="A148" s="30" t="s">
         <v>169</v>
       </c>
@@ -7372,7 +7365,7 @@
       </c>
       <c r="I151" s="32"/>
     </row>
-    <row r="152" spans="1:9" hidden="1">
+    <row r="152" spans="1:9">
       <c r="A152" s="30" t="s">
         <v>173</v>
       </c>
@@ -7555,7 +7548,7 @@
       </c>
       <c r="I158" s="32"/>
     </row>
-    <row r="159" spans="1:9" hidden="1">
+    <row r="159" spans="1:9">
       <c r="A159" s="30" t="s">
         <v>180</v>
       </c>
@@ -7580,7 +7573,7 @@
       </c>
       <c r="I159" s="32"/>
     </row>
-    <row r="160" spans="1:9" ht="30" hidden="1">
+    <row r="160" spans="1:9" ht="30">
       <c r="A160" s="30" t="s">
         <v>181</v>
       </c>
@@ -7680,7 +7673,7 @@
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" ht="30">
       <c r="A164" s="30" t="s">
         <v>185</v>
       </c>
@@ -7780,7 +7773,7 @@
       </c>
       <c r="I167" s="32"/>
     </row>
-    <row r="168" spans="1:9" ht="30" hidden="1">
+    <row r="168" spans="1:9" ht="30">
       <c r="A168" s="30" t="s">
         <v>189</v>
       </c>
@@ -7805,7 +7798,7 @@
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="30" hidden="1">
+    <row r="169" spans="1:9" ht="30">
       <c r="A169" s="30" t="s">
         <v>190</v>
       </c>
@@ -7830,7 +7823,7 @@
       </c>
       <c r="I169" s="32"/>
     </row>
-    <row r="170" spans="1:9" hidden="1">
+    <row r="170" spans="1:9">
       <c r="A170" s="30" t="s">
         <v>191</v>
       </c>
@@ -7982,7 +7975,7 @@
       </c>
       <c r="I175" s="32"/>
     </row>
-    <row r="176" spans="1:9" ht="30" hidden="1">
+    <row r="176" spans="1:9" ht="30">
       <c r="A176" s="30" t="s">
         <v>196</v>
       </c>
@@ -8057,7 +8050,7 @@
       </c>
       <c r="I178" s="32"/>
     </row>
-    <row r="179" spans="1:9" ht="30" hidden="1">
+    <row r="179" spans="1:9" ht="30">
       <c r="A179" s="30" t="s">
         <v>199</v>
       </c>
@@ -8157,7 +8150,7 @@
       </c>
       <c r="I182" s="32"/>
     </row>
-    <row r="183" spans="1:9" hidden="1">
+    <row r="183" spans="1:9">
       <c r="A183" s="30" t="s">
         <v>203</v>
       </c>
@@ -8232,7 +8225,7 @@
       </c>
       <c r="I185" s="32"/>
     </row>
-    <row r="186" spans="1:9" ht="30" hidden="1">
+    <row r="186" spans="1:9" ht="30">
       <c r="A186" s="30" t="s">
         <v>206</v>
       </c>
@@ -8307,7 +8300,7 @@
       </c>
       <c r="I188" s="32"/>
     </row>
-    <row r="189" spans="1:9" hidden="1">
+    <row r="189" spans="1:9">
       <c r="A189" s="30" t="s">
         <v>209</v>
       </c>
@@ -8382,7 +8375,7 @@
       </c>
       <c r="I191" s="32"/>
     </row>
-    <row r="192" spans="1:9" ht="30" hidden="1">
+    <row r="192" spans="1:9" ht="30">
       <c r="A192" s="30" t="s">
         <v>212</v>
       </c>
@@ -8432,7 +8425,7 @@
       </c>
       <c r="I193" s="32"/>
     </row>
-    <row r="194" spans="1:9" ht="30" hidden="1">
+    <row r="194" spans="1:9" ht="30">
       <c r="A194" s="30" t="s">
         <v>214</v>
       </c>
@@ -8457,7 +8450,7 @@
       </c>
       <c r="I194" s="32"/>
     </row>
-    <row r="195" spans="1:9" hidden="1">
+    <row r="195" spans="1:9">
       <c r="A195" s="30" t="s">
         <v>215</v>
       </c>
@@ -8507,7 +8500,7 @@
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" ht="30">
       <c r="A197" s="30" t="s">
         <v>217</v>
       </c>
@@ -8557,7 +8550,7 @@
       </c>
       <c r="I198" s="32"/>
     </row>
-    <row r="199" spans="1:9" hidden="1">
+    <row r="199" spans="1:9">
       <c r="A199" s="30" t="s">
         <v>219</v>
       </c>
@@ -8582,7 +8575,7 @@
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="30">
+    <row r="200" spans="1:9" ht="45">
       <c r="A200" s="30" t="s">
         <v>220</v>
       </c>
@@ -8607,7 +8600,7 @@
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="45" hidden="1">
+    <row r="201" spans="1:9" ht="45">
       <c r="A201" s="30" t="s">
         <v>221</v>
       </c>
@@ -8632,7 +8625,7 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9" ht="30" hidden="1">
+    <row r="202" spans="1:9" ht="30">
       <c r="A202" s="30" t="s">
         <v>222</v>
       </c>
@@ -8782,7 +8775,7 @@
       </c>
       <c r="I207" s="32"/>
     </row>
-    <row r="208" spans="1:9" hidden="1">
+    <row r="208" spans="1:9">
       <c r="A208" s="30" t="s">
         <v>228</v>
       </c>
@@ -9057,7 +9050,7 @@
       </c>
       <c r="I218" s="32"/>
     </row>
-    <row r="219" spans="1:9" ht="45">
+    <row r="219" spans="1:9" ht="60">
       <c r="A219" s="22" t="s">
         <v>239</v>
       </c>
@@ -9184,7 +9177,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1">
+    <row r="224" spans="1:9">
       <c r="A224" s="30" t="s">
         <v>244</v>
       </c>
@@ -9209,7 +9202,7 @@
       </c>
       <c r="I224" s="32"/>
     </row>
-    <row r="225" spans="1:9" ht="30" hidden="1">
+    <row r="225" spans="1:9" ht="30">
       <c r="A225" s="30" t="s">
         <v>245</v>
       </c>
@@ -9309,7 +9302,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" ht="30">
       <c r="A229" s="30" t="s">
         <v>249</v>
       </c>
@@ -9359,7 +9352,7 @@
       </c>
       <c r="I230" s="32"/>
     </row>
-    <row r="231" spans="1:9" ht="165">
+    <row r="231" spans="1:9" ht="180">
       <c r="A231" s="30" t="s">
         <v>251</v>
       </c>
@@ -9384,7 +9377,7 @@
       </c>
       <c r="I231" s="32"/>
     </row>
-    <row r="232" spans="1:9" hidden="1">
+    <row r="232" spans="1:9">
       <c r="A232" s="30" t="s">
         <v>252</v>
       </c>
@@ -9409,7 +9402,7 @@
       </c>
       <c r="I232" s="32"/>
     </row>
-    <row r="233" spans="1:9" hidden="1">
+    <row r="233" spans="1:9">
       <c r="A233" s="30" t="s">
         <v>253</v>
       </c>
@@ -9434,7 +9427,7 @@
       </c>
       <c r="I233" s="32"/>
     </row>
-    <row r="234" spans="1:9" ht="30" hidden="1">
+    <row r="234" spans="1:9" ht="30">
       <c r="A234" s="30" t="s">
         <v>254</v>
       </c>
@@ -9484,7 +9477,7 @@
       </c>
       <c r="I235" s="32"/>
     </row>
-    <row r="236" spans="1:9" ht="30" hidden="1">
+    <row r="236" spans="1:9" ht="30">
       <c r="A236" s="30" t="s">
         <v>256</v>
       </c>
@@ -9559,7 +9552,7 @@
       </c>
       <c r="I238" s="32"/>
     </row>
-    <row r="239" spans="1:9" ht="30" hidden="1">
+    <row r="239" spans="1:9" ht="30">
       <c r="A239" s="30" t="s">
         <v>259</v>
       </c>
@@ -9584,7 +9577,7 @@
       </c>
       <c r="I239" s="32"/>
     </row>
-    <row r="240" spans="1:9" hidden="1">
+    <row r="240" spans="1:9">
       <c r="A240" s="30" t="s">
         <v>260</v>
       </c>
@@ -9609,7 +9602,7 @@
       </c>
       <c r="I240" s="32"/>
     </row>
-    <row r="241" spans="1:9" ht="30" hidden="1">
+    <row r="241" spans="1:9" ht="30">
       <c r="A241" s="30" t="s">
         <v>261</v>
       </c>
@@ -9684,7 +9677,7 @@
       </c>
       <c r="I243" s="32"/>
     </row>
-    <row r="244" spans="1:9" hidden="1">
+    <row r="244" spans="1:9">
       <c r="A244" s="30" t="s">
         <v>264</v>
       </c>
@@ -9759,7 +9752,7 @@
       </c>
       <c r="I246" s="32"/>
     </row>
-    <row r="247" spans="1:9" hidden="1">
+    <row r="247" spans="1:9">
       <c r="A247" s="30" t="s">
         <v>267</v>
       </c>
@@ -9834,7 +9827,7 @@
       </c>
       <c r="I249" s="32"/>
     </row>
-    <row r="250" spans="1:9" ht="30" hidden="1">
+    <row r="250" spans="1:9" ht="30">
       <c r="A250" s="30" t="s">
         <v>270</v>
       </c>
@@ -9859,7 +9852,7 @@
       </c>
       <c r="I250" s="32"/>
     </row>
-    <row r="251" spans="1:9" ht="30" hidden="1">
+    <row r="251" spans="1:9" ht="30">
       <c r="A251" s="30" t="s">
         <v>271</v>
       </c>
@@ -9884,7 +9877,7 @@
       </c>
       <c r="I251" s="32"/>
     </row>
-    <row r="252" spans="1:9" hidden="1">
+    <row r="252" spans="1:9">
       <c r="A252" s="30" t="s">
         <v>272</v>
       </c>
@@ -10009,7 +10002,7 @@
       </c>
       <c r="I256" s="32"/>
     </row>
-    <row r="257" spans="1:9" ht="30" hidden="1">
+    <row r="257" spans="1:9" ht="30">
       <c r="A257" s="30" t="s">
         <v>277</v>
       </c>
@@ -10059,7 +10052,7 @@
       </c>
       <c r="I258" s="32"/>
     </row>
-    <row r="259" spans="1:9" ht="45">
+    <row r="259" spans="1:9" ht="60">
       <c r="A259" s="22" t="s">
         <v>279</v>
       </c>
@@ -10134,7 +10127,7 @@
       </c>
       <c r="I261" s="32"/>
     </row>
-    <row r="262" spans="1:9" ht="30" hidden="1">
+    <row r="262" spans="1:9" ht="30">
       <c r="A262" s="30" t="s">
         <v>282</v>
       </c>
@@ -10423,7 +10416,7 @@
       </c>
       <c r="I272" s="32"/>
     </row>
-    <row r="273" spans="1:9" ht="45">
+    <row r="273" spans="1:9" ht="60">
       <c r="A273" s="30" t="s">
         <v>293</v>
       </c>
@@ -10450,7 +10443,7 @@
       </c>
       <c r="I273" s="32"/>
     </row>
-    <row r="274" spans="1:9" ht="30" hidden="1">
+    <row r="274" spans="1:9" ht="30">
       <c r="A274" s="30" t="s">
         <v>294</v>
       </c>
@@ -10600,7 +10593,7 @@
       </c>
       <c r="I279" s="32"/>
     </row>
-    <row r="280" spans="1:9" ht="135">
+    <row r="280" spans="1:9" ht="150">
       <c r="A280" s="30" t="s">
         <v>300</v>
       </c>
@@ -10625,7 +10618,7 @@
       </c>
       <c r="I280" s="32"/>
     </row>
-    <row r="281" spans="1:9" hidden="1">
+    <row r="281" spans="1:9">
       <c r="A281" s="30" t="s">
         <v>301</v>
       </c>
@@ -10750,7 +10743,7 @@
       </c>
       <c r="I285" s="32"/>
     </row>
-    <row r="286" spans="1:9" ht="30" hidden="1">
+    <row r="286" spans="1:9" ht="30">
       <c r="A286" s="30" t="s">
         <v>306</v>
       </c>
@@ -10800,7 +10793,7 @@
       </c>
       <c r="I287" s="32"/>
     </row>
-    <row r="288" spans="1:9">
+    <row r="288" spans="1:9" ht="30">
       <c r="A288" s="30" t="s">
         <v>308</v>
       </c>
@@ -10875,7 +10868,7 @@
       </c>
       <c r="I290" s="32"/>
     </row>
-    <row r="291" spans="1:9" hidden="1">
+    <row r="291" spans="1:9">
       <c r="A291" s="30" t="s">
         <v>311</v>
       </c>
@@ -11354,7 +11347,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="308" spans="1:9" ht="45" hidden="1">
+    <row r="308" spans="1:9" ht="45">
       <c r="A308" s="22" t="s">
         <v>323</v>
       </c>
@@ -11379,7 +11372,7 @@
       </c>
       <c r="I308" s="32"/>
     </row>
-    <row r="309" spans="1:9" ht="30" hidden="1">
+    <row r="309" spans="1:9" ht="30">
       <c r="A309" s="30" t="s">
         <v>324</v>
       </c>
@@ -11492,12 +11485,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -11546,16 +11548,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -11569,7 +11570,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11582,12 +11583,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-COPYS] Add new case about "Unknouw" error in CopyIntoItemsLocal and update capture codes.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2279EE-E836-4FB3-8DD5-73E29548F8A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2082920-71AE-40D6-A5D1-B2A3129758B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-2085" windowWidth="24240" windowHeight="13290" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$304</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$305</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2106" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="691">
   <si>
     <t>Req ID</t>
   </si>
@@ -2416,9 +2416,6 @@
     <t>[In CopyIntoItems] If the file cannot be created at the given destination location, the protocol server MUST report a failure for this destination location by setting the ErrorCode attribute of the corresponding CopyResult element to "Unknown" and provide a string value that describes the error in the ErrorMessage attribute.</t>
   </si>
   <si>
-    <t>[In CopyIntoItemsLocal] If the source location does not point to an existing file, then if the destination location does not point to a existing folder or file, the protocol server MUST report a failure by returning the CopyResult element (section 2.2.4.2) with the ErrorCode attribute set to "Unknown" for this destination location.</t>
-  </si>
-  <si>
     <t xml:space="preserve">[In CopyIntoItemsLocal] If the source location does not point to an existing file, then if the destination location points to an existing file, the protocol server MUST report a failure by returning the CopyResult element with the ErrorCode attribute set to "SourceInvalid" for this destination location. </t>
   </si>
   <si>
@@ -2459,6 +2456,22 @@
   </si>
   <si>
     <t>[In CopyIntoItemsLocal] If the source location points to a file whose permission setting does not allow access by the protocol client, then if the destination location points to an existing file whose permission setting does not allow access by the protocol client, the protocol server MUST report a failure by returning the CopyResult element with the ErrorCode attribute set to "Unknown" for this destination location.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-COPYS_R271002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.4.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In CopyIntoItemsLocal] If the source location does not point to an existing file, then if the destination location does not point to a existing folder or file, the protocol server MUST report a failure by returning the CopyResult element (section 2.2.4.2) with the ErrorCode attribute set to "Unknown" for this destination location.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In CopyIntoItemsLocal] If the source location does not point to an existing file, then if the destination location points to an existing file whose permission setting does not allow access by the protocol client, the protocol server MUST report a failure by returning the CopyResult element with the ErrorCode attribute set to "Unknown" for this destination location.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2520,6 +2533,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2738,6 +2752,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2777,61 +2797,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3170,6 +3140,50 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3299,34 +3313,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I304" tableType="xml" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" connectionId="1">
-  <autoFilter ref="A19:I304" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I305" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I305" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="3.1.4.3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="23">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="22">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="21">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="16">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3335,12 +3355,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3668,13 +3688,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L306"/>
+  <dimension ref="A1:L307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
@@ -3724,127 +3744,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3857,12 +3877,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3875,12 +3895,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3893,12 +3913,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3911,60 +3931,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3998,7 +4018,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
@@ -4023,7 +4043,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -4050,7 +4070,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -4075,7 +4095,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="s">
         <v>46</v>
       </c>
@@ -4083,7 +4103,7 @@
         <v>317</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -4100,7 +4120,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="s">
         <v>47</v>
       </c>
@@ -4125,7 +4145,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
@@ -4133,7 +4153,7 @@
         <v>317</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -4150,7 +4170,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -4175,7 +4195,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -4200,7 +4220,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -4225,7 +4245,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
@@ -4250,7 +4270,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="s">
         <v>53</v>
       </c>
@@ -4275,7 +4295,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -4300,7 +4320,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -4325,7 +4345,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
@@ -4350,7 +4370,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>57</v>
       </c>
@@ -4375,7 +4395,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>58</v>
       </c>
@@ -4400,7 +4420,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>59</v>
       </c>
@@ -4425,7 +4445,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>60</v>
       </c>
@@ -4450,7 +4470,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>61</v>
       </c>
@@ -4475,7 +4495,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>
@@ -4500,7 +4520,7 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>63</v>
       </c>
@@ -4525,7 +4545,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>64</v>
       </c>
@@ -4550,7 +4570,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>65</v>
       </c>
@@ -4575,7 +4595,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>66</v>
       </c>
@@ -4600,7 +4620,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>67</v>
       </c>
@@ -4625,7 +4645,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
         <v>68</v>
       </c>
@@ -4650,7 +4670,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>69</v>
       </c>
@@ -4675,7 +4695,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>70</v>
       </c>
@@ -4700,7 +4720,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>71</v>
       </c>
@@ -4725,7 +4745,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>72</v>
       </c>
@@ -4750,7 +4770,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>73</v>
       </c>
@@ -4775,7 +4795,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>74</v>
       </c>
@@ -4800,7 +4820,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>75</v>
       </c>
@@ -4825,7 +4845,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>76</v>
       </c>
@@ -4850,7 +4870,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>77</v>
       </c>
@@ -4875,7 +4895,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>78</v>
       </c>
@@ -4900,7 +4920,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
         <v>79</v>
       </c>
@@ -4925,7 +4945,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>80</v>
       </c>
@@ -4950,7 +4970,7 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
         <v>81</v>
       </c>
@@ -4975,7 +4995,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
         <v>82</v>
       </c>
@@ -5000,7 +5020,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>83</v>
       </c>
@@ -5027,7 +5047,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>84</v>
       </c>
@@ -5054,7 +5074,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>85</v>
       </c>
@@ -5079,7 +5099,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>86</v>
       </c>
@@ -5106,7 +5126,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>87</v>
       </c>
@@ -5133,7 +5153,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>88</v>
       </c>
@@ -5158,7 +5178,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>89</v>
       </c>
@@ -5183,7 +5203,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>90</v>
       </c>
@@ -5208,7 +5228,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>91</v>
       </c>
@@ -5233,7 +5253,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>92</v>
       </c>
@@ -5258,7 +5278,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>93</v>
       </c>
@@ -5283,7 +5303,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>94</v>
       </c>
@@ -5308,7 +5328,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>95</v>
       </c>
@@ -5333,7 +5353,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>96</v>
       </c>
@@ -5358,7 +5378,7 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>97</v>
       </c>
@@ -5383,7 +5403,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>98</v>
       </c>
@@ -5408,7 +5428,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>99</v>
       </c>
@@ -5433,7 +5453,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>100</v>
       </c>
@@ -5458,7 +5478,7 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>101</v>
       </c>
@@ -5483,7 +5503,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>102</v>
       </c>
@@ -5508,7 +5528,7 @@
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>103</v>
       </c>
@@ -5533,7 +5553,7 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>104</v>
       </c>
@@ -5558,7 +5578,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>105</v>
       </c>
@@ -5585,7 +5605,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>106</v>
       </c>
@@ -5612,7 +5632,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>107</v>
       </c>
@@ -5639,7 +5659,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
         <v>108</v>
       </c>
@@ -5666,7 +5686,7 @@
       </c>
       <c r="I85" s="32"/>
     </row>
-    <row r="86" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>109</v>
       </c>
@@ -5691,7 +5711,7 @@
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>110</v>
       </c>
@@ -5716,7 +5736,7 @@
       </c>
       <c r="I87" s="32"/>
     </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
         <v>111</v>
       </c>
@@ -5741,7 +5761,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
         <v>112</v>
       </c>
@@ -5766,7 +5786,7 @@
       </c>
       <c r="I89" s="32"/>
     </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
         <v>113</v>
       </c>
@@ -5791,7 +5811,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
         <v>114</v>
       </c>
@@ -5816,7 +5836,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
         <v>115</v>
       </c>
@@ -5841,7 +5861,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
         <v>116</v>
       </c>
@@ -5866,7 +5886,7 @@
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>117</v>
       </c>
@@ -5891,7 +5911,7 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
         <v>118</v>
       </c>
@@ -5916,7 +5936,7 @@
       </c>
       <c r="I95" s="32"/>
     </row>
-    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
         <v>119</v>
       </c>
@@ -5941,7 +5961,7 @@
       </c>
       <c r="I96" s="32"/>
     </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
         <v>120</v>
       </c>
@@ -5968,7 +5988,7 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
         <v>121</v>
       </c>
@@ -5995,7 +6015,7 @@
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
         <v>122</v>
       </c>
@@ -6020,7 +6040,7 @@
       </c>
       <c r="I99" s="32"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
         <v>123</v>
       </c>
@@ -6045,7 +6065,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
         <v>124</v>
       </c>
@@ -6070,7 +6090,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
         <v>125</v>
       </c>
@@ -6097,7 +6117,7 @@
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="30" t="s">
         <v>126</v>
       </c>
@@ -6124,7 +6144,7 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="30" t="s">
         <v>127</v>
       </c>
@@ -6149,7 +6169,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
         <v>128</v>
       </c>
@@ -6174,7 +6194,7 @@
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="30" t="s">
         <v>129</v>
       </c>
@@ -6201,7 +6221,7 @@
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="30" t="s">
         <v>130</v>
       </c>
@@ -6228,7 +6248,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22" t="s">
         <v>131</v>
       </c>
@@ -6253,7 +6273,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="30" t="s">
         <v>132</v>
       </c>
@@ -6278,7 +6298,7 @@
       </c>
       <c r="I109" s="32"/>
     </row>
-    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="30" t="s">
         <v>133</v>
       </c>
@@ -6305,7 +6325,7 @@
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="30" t="s">
         <v>134</v>
       </c>
@@ -6332,7 +6352,7 @@
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="30" t="s">
         <v>135</v>
       </c>
@@ -6357,7 +6377,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="30" t="s">
         <v>136</v>
       </c>
@@ -6382,7 +6402,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="30" t="s">
         <v>137</v>
       </c>
@@ -6407,7 +6427,7 @@
       </c>
       <c r="I114" s="32"/>
     </row>
-    <row r="115" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
         <v>138</v>
       </c>
@@ -6434,7 +6454,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="30" t="s">
         <v>139</v>
       </c>
@@ -6461,7 +6481,7 @@
       </c>
       <c r="I116" s="32"/>
     </row>
-    <row r="117" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22" t="s">
         <v>140</v>
       </c>
@@ -6488,7 +6508,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="22" t="s">
         <v>644</v>
       </c>
@@ -6513,7 +6533,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22" t="s">
         <v>646</v>
       </c>
@@ -6538,7 +6558,7 @@
       </c>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="30" t="s">
         <v>141</v>
       </c>
@@ -6563,7 +6583,7 @@
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
         <v>142</v>
       </c>
@@ -6588,7 +6608,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="30" t="s">
         <v>143</v>
       </c>
@@ -6613,7 +6633,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="30" t="s">
         <v>144</v>
       </c>
@@ -6638,7 +6658,7 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="30" t="s">
         <v>145</v>
       </c>
@@ -6663,7 +6683,7 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="30" t="s">
         <v>146</v>
       </c>
@@ -6688,7 +6708,7 @@
       </c>
       <c r="I125" s="32"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="30" t="s">
         <v>147</v>
       </c>
@@ -6713,7 +6733,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="30" t="s">
         <v>148</v>
       </c>
@@ -6738,7 +6758,7 @@
       </c>
       <c r="I127" s="32"/>
     </row>
-    <row r="128" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="30" t="s">
         <v>149</v>
       </c>
@@ -6763,7 +6783,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="30" t="s">
         <v>150</v>
       </c>
@@ -6788,7 +6808,7 @@
       </c>
       <c r="I129" s="32"/>
     </row>
-    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="30" t="s">
         <v>151</v>
       </c>
@@ -6813,7 +6833,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="30" t="s">
         <v>152</v>
       </c>
@@ -6838,7 +6858,7 @@
       </c>
       <c r="I131" s="32"/>
     </row>
-    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="30" t="s">
         <v>153</v>
       </c>
@@ -6863,7 +6883,7 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="30" t="s">
         <v>154</v>
       </c>
@@ -6888,7 +6908,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="30" t="s">
         <v>155</v>
       </c>
@@ -6913,7 +6933,7 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="30" t="s">
         <v>156</v>
       </c>
@@ -6938,7 +6958,7 @@
       </c>
       <c r="I135" s="32"/>
     </row>
-    <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="30" t="s">
         <v>157</v>
       </c>
@@ -6963,7 +6983,7 @@
       </c>
       <c r="I136" s="32"/>
     </row>
-    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="30" t="s">
         <v>158</v>
       </c>
@@ -6988,7 +7008,7 @@
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="30" t="s">
         <v>159</v>
       </c>
@@ -7013,7 +7033,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="30" t="s">
         <v>160</v>
       </c>
@@ -7040,7 +7060,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="30" t="s">
         <v>161</v>
       </c>
@@ -7065,7 +7085,7 @@
       </c>
       <c r="I140" s="32"/>
     </row>
-    <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="30" t="s">
         <v>162</v>
       </c>
@@ -7090,7 +7110,7 @@
       </c>
       <c r="I141" s="32"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="30" t="s">
         <v>163</v>
       </c>
@@ -7115,7 +7135,7 @@
       </c>
       <c r="I142" s="32"/>
     </row>
-    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="30" t="s">
         <v>164</v>
       </c>
@@ -7140,7 +7160,7 @@
       </c>
       <c r="I143" s="32"/>
     </row>
-    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="30" t="s">
         <v>165</v>
       </c>
@@ -7167,7 +7187,7 @@
       </c>
       <c r="I144" s="32"/>
     </row>
-    <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="30" t="s">
         <v>166</v>
       </c>
@@ -7194,7 +7214,7 @@
       </c>
       <c r="I145" s="32"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="30" t="s">
         <v>167</v>
       </c>
@@ -7219,7 +7239,7 @@
       </c>
       <c r="I146" s="32"/>
     </row>
-    <row r="147" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="30" t="s">
         <v>168</v>
       </c>
@@ -7244,7 +7264,7 @@
       </c>
       <c r="I147" s="32"/>
     </row>
-    <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="30" t="s">
         <v>169</v>
       </c>
@@ -7271,7 +7291,7 @@
       </c>
       <c r="I148" s="32"/>
     </row>
-    <row r="149" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="30" t="s">
         <v>170</v>
       </c>
@@ -7298,7 +7318,7 @@
       </c>
       <c r="I149" s="32"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="30" t="s">
         <v>171</v>
       </c>
@@ -7323,7 +7343,7 @@
       </c>
       <c r="I150" s="32"/>
     </row>
-    <row r="151" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="30" t="s">
         <v>172</v>
       </c>
@@ -7350,7 +7370,7 @@
       </c>
       <c r="I151" s="32"/>
     </row>
-    <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="30" t="s">
         <v>173</v>
       </c>
@@ -7377,7 +7397,7 @@
       </c>
       <c r="I152" s="32"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="30" t="s">
         <v>174</v>
       </c>
@@ -7402,7 +7422,7 @@
       </c>
       <c r="I153" s="32"/>
     </row>
-    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="30" t="s">
         <v>175</v>
       </c>
@@ -7427,7 +7447,7 @@
       </c>
       <c r="I154" s="32"/>
     </row>
-    <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="30" t="s">
         <v>176</v>
       </c>
@@ -7452,7 +7472,7 @@
       </c>
       <c r="I155" s="32"/>
     </row>
-    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="30" t="s">
         <v>177</v>
       </c>
@@ -7477,7 +7497,7 @@
       </c>
       <c r="I156" s="32"/>
     </row>
-    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="30" t="s">
         <v>178</v>
       </c>
@@ -7502,7 +7522,7 @@
       </c>
       <c r="I157" s="32"/>
     </row>
-    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="30" t="s">
         <v>179</v>
       </c>
@@ -7527,7 +7547,7 @@
       </c>
       <c r="I158" s="32"/>
     </row>
-    <row r="159" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="30" t="s">
         <v>180</v>
       </c>
@@ -7552,7 +7572,7 @@
       </c>
       <c r="I159" s="32"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="30" t="s">
         <v>181</v>
       </c>
@@ -7577,7 +7597,7 @@
       </c>
       <c r="I160" s="32"/>
     </row>
-    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="30" t="s">
         <v>182</v>
       </c>
@@ -7602,7 +7622,7 @@
       </c>
       <c r="I161" s="32"/>
     </row>
-    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="30" t="s">
         <v>183</v>
       </c>
@@ -7627,7 +7647,7 @@
       </c>
       <c r="I162" s="32"/>
     </row>
-    <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="30" t="s">
         <v>184</v>
       </c>
@@ -7652,7 +7672,7 @@
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="30" t="s">
         <v>185</v>
       </c>
@@ -7677,7 +7697,7 @@
       </c>
       <c r="I164" s="32"/>
     </row>
-    <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="22" t="s">
         <v>654</v>
       </c>
@@ -7701,10 +7721,10 @@
         <v>17</v>
       </c>
       <c r="I165" s="20" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="30" t="s">
         <v>186</v>
       </c>
@@ -7729,7 +7749,7 @@
       </c>
       <c r="I166" s="32"/>
     </row>
-    <row r="167" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="30" t="s">
         <v>187</v>
       </c>
@@ -7754,7 +7774,7 @@
       </c>
       <c r="I167" s="32"/>
     </row>
-    <row r="168" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="30" t="s">
         <v>188</v>
       </c>
@@ -7779,7 +7799,7 @@
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="30" t="s">
         <v>189</v>
       </c>
@@ -7804,7 +7824,7 @@
       </c>
       <c r="I169" s="32"/>
     </row>
-    <row r="170" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="30" t="s">
         <v>190</v>
       </c>
@@ -7829,7 +7849,7 @@
       </c>
       <c r="I170" s="32"/>
     </row>
-    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="30" t="s">
         <v>191</v>
       </c>
@@ -7854,7 +7874,7 @@
       </c>
       <c r="I171" s="32"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="30" t="s">
         <v>192</v>
       </c>
@@ -7879,7 +7899,7 @@
       </c>
       <c r="I172" s="32"/>
     </row>
-    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="30" t="s">
         <v>193</v>
       </c>
@@ -7904,7 +7924,7 @@
       </c>
       <c r="I173" s="32"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="30" t="s">
         <v>194</v>
       </c>
@@ -7929,7 +7949,7 @@
       </c>
       <c r="I174" s="32"/>
     </row>
-    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="30" t="s">
         <v>195</v>
       </c>
@@ -7954,7 +7974,7 @@
       </c>
       <c r="I175" s="32"/>
     </row>
-    <row r="176" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="30" t="s">
         <v>196</v>
       </c>
@@ -7979,7 +7999,7 @@
       </c>
       <c r="I176" s="32"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="30" t="s">
         <v>197</v>
       </c>
@@ -8004,7 +8024,7 @@
       </c>
       <c r="I177" s="32"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="30" t="s">
         <v>198</v>
       </c>
@@ -8029,7 +8049,7 @@
       </c>
       <c r="I178" s="32"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="30" t="s">
         <v>199</v>
       </c>
@@ -8054,7 +8074,7 @@
       </c>
       <c r="I179" s="32"/>
     </row>
-    <row r="180" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="30" t="s">
         <v>200</v>
       </c>
@@ -8079,7 +8099,7 @@
       </c>
       <c r="I180" s="32"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="30" t="s">
         <v>201</v>
       </c>
@@ -8104,7 +8124,7 @@
       </c>
       <c r="I181" s="32"/>
     </row>
-    <row r="182" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="30" t="s">
         <v>202</v>
       </c>
@@ -8129,7 +8149,7 @@
       </c>
       <c r="I182" s="32"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="30" t="s">
         <v>203</v>
       </c>
@@ -8154,7 +8174,7 @@
       </c>
       <c r="I183" s="32"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="30" t="s">
         <v>204</v>
       </c>
@@ -8179,7 +8199,7 @@
       </c>
       <c r="I184" s="32"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="30" t="s">
         <v>205</v>
       </c>
@@ -8204,7 +8224,7 @@
       </c>
       <c r="I185" s="32"/>
     </row>
-    <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="30" t="s">
         <v>206</v>
       </c>
@@ -8229,7 +8249,7 @@
       </c>
       <c r="I186" s="32"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="30" t="s">
         <v>207</v>
       </c>
@@ -8254,7 +8274,7 @@
       </c>
       <c r="I187" s="32"/>
     </row>
-    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="30" t="s">
         <v>208</v>
       </c>
@@ -8279,7 +8299,7 @@
       </c>
       <c r="I188" s="32"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="30" t="s">
         <v>209</v>
       </c>
@@ -8304,7 +8324,7 @@
       </c>
       <c r="I189" s="32"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="30" t="s">
         <v>210</v>
       </c>
@@ -8329,7 +8349,7 @@
       </c>
       <c r="I190" s="32"/>
     </row>
-    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="30" t="s">
         <v>211</v>
       </c>
@@ -8354,7 +8374,7 @@
       </c>
       <c r="I191" s="32"/>
     </row>
-    <row r="192" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="30" t="s">
         <v>212</v>
       </c>
@@ -8379,7 +8399,7 @@
       </c>
       <c r="I192" s="32"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="30" t="s">
         <v>213</v>
       </c>
@@ -8404,7 +8424,7 @@
       </c>
       <c r="I193" s="32"/>
     </row>
-    <row r="194" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="30" t="s">
         <v>214</v>
       </c>
@@ -8429,7 +8449,7 @@
       </c>
       <c r="I194" s="32"/>
     </row>
-    <row r="195" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="30" t="s">
         <v>215</v>
       </c>
@@ -8454,7 +8474,7 @@
       </c>
       <c r="I195" s="32"/>
     </row>
-    <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="30" t="s">
         <v>216</v>
       </c>
@@ -8479,7 +8499,7 @@
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="30" t="s">
         <v>217</v>
       </c>
@@ -8504,7 +8524,7 @@
       </c>
       <c r="I197" s="32"/>
     </row>
-    <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="30" t="s">
         <v>218</v>
       </c>
@@ -8529,7 +8549,7 @@
       </c>
       <c r="I198" s="32"/>
     </row>
-    <row r="199" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="30" t="s">
         <v>219</v>
       </c>
@@ -8554,7 +8574,7 @@
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="30" t="s">
         <v>220</v>
       </c>
@@ -8579,7 +8599,7 @@
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="30" t="s">
         <v>221</v>
       </c>
@@ -8604,7 +8624,7 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="30" t="s">
         <v>222</v>
       </c>
@@ -8629,7 +8649,7 @@
       </c>
       <c r="I202" s="32"/>
     </row>
-    <row r="203" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="30" t="s">
         <v>223</v>
       </c>
@@ -8654,7 +8674,7 @@
       </c>
       <c r="I203" s="32"/>
     </row>
-    <row r="204" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="30" t="s">
         <v>224</v>
       </c>
@@ -8679,7 +8699,7 @@
       </c>
       <c r="I204" s="32"/>
     </row>
-    <row r="205" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="30" t="s">
         <v>225</v>
       </c>
@@ -8704,7 +8724,7 @@
       </c>
       <c r="I205" s="32"/>
     </row>
-    <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="30" t="s">
         <v>226</v>
       </c>
@@ -8729,7 +8749,7 @@
       </c>
       <c r="I206" s="32"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="30" t="s">
         <v>227</v>
       </c>
@@ -8754,7 +8774,7 @@
       </c>
       <c r="I207" s="32"/>
     </row>
-    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="30" t="s">
         <v>228</v>
       </c>
@@ -8779,7 +8799,7 @@
       </c>
       <c r="I208" s="32"/>
     </row>
-    <row r="209" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="30" t="s">
         <v>229</v>
       </c>
@@ -8804,7 +8824,7 @@
       </c>
       <c r="I209" s="32"/>
     </row>
-    <row r="210" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="30" t="s">
         <v>230</v>
       </c>
@@ -8829,7 +8849,7 @@
       </c>
       <c r="I210" s="32"/>
     </row>
-    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="30" t="s">
         <v>231</v>
       </c>
@@ -8854,7 +8874,7 @@
       </c>
       <c r="I211" s="32"/>
     </row>
-    <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="30" t="s">
         <v>232</v>
       </c>
@@ -8879,7 +8899,7 @@
       </c>
       <c r="I212" s="32"/>
     </row>
-    <row r="213" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="22" t="s">
         <v>233</v>
       </c>
@@ -8904,7 +8924,7 @@
       </c>
       <c r="I213" s="32"/>
     </row>
-    <row r="214" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="30" t="s">
         <v>234</v>
       </c>
@@ -8929,7 +8949,7 @@
       </c>
       <c r="I214" s="32"/>
     </row>
-    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="30" t="s">
         <v>235</v>
       </c>
@@ -8954,7 +8974,7 @@
       </c>
       <c r="I215" s="32"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="30" t="s">
         <v>236</v>
       </c>
@@ -8979,7 +8999,7 @@
       </c>
       <c r="I216" s="32"/>
     </row>
-    <row r="217" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="22" t="s">
         <v>237</v>
       </c>
@@ -9006,7 +9026,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="30" t="s">
         <v>238</v>
       </c>
@@ -9031,7 +9051,7 @@
       </c>
       <c r="I218" s="32"/>
     </row>
-    <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="30" t="s">
         <v>239</v>
       </c>
@@ -9056,7 +9076,7 @@
       </c>
       <c r="I219" s="32"/>
     </row>
-    <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="30" t="s">
         <v>240</v>
       </c>
@@ -9081,7 +9101,7 @@
       </c>
       <c r="I220" s="32"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="30" t="s">
         <v>241</v>
       </c>
@@ -9106,7 +9126,7 @@
       </c>
       <c r="I221" s="32"/>
     </row>
-    <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="30" t="s">
         <v>242</v>
       </c>
@@ -9131,7 +9151,7 @@
       </c>
       <c r="I222" s="32"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="30" t="s">
         <v>243</v>
       </c>
@@ -9156,7 +9176,7 @@
       </c>
       <c r="I223" s="32"/>
     </row>
-    <row r="224" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="30" t="s">
         <v>244</v>
       </c>
@@ -9181,7 +9201,7 @@
       </c>
       <c r="I224" s="32"/>
     </row>
-    <row r="225" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="30" t="s">
         <v>245</v>
       </c>
@@ -9206,7 +9226,7 @@
       </c>
       <c r="I225" s="32"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="30" t="s">
         <v>246</v>
       </c>
@@ -9231,7 +9251,7 @@
       </c>
       <c r="I226" s="32"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="30" t="s">
         <v>247</v>
       </c>
@@ -9256,7 +9276,7 @@
       </c>
       <c r="I227" s="32"/>
     </row>
-    <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="30" t="s">
         <v>248</v>
       </c>
@@ -9281,7 +9301,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="30" t="s">
         <v>249</v>
       </c>
@@ -9306,7 +9326,7 @@
       </c>
       <c r="I229" s="32"/>
     </row>
-    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="30" t="s">
         <v>250</v>
       </c>
@@ -9331,7 +9351,7 @@
       </c>
       <c r="I230" s="32"/>
     </row>
-    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="30" t="s">
         <v>251</v>
       </c>
@@ -9356,7 +9376,7 @@
       </c>
       <c r="I231" s="32"/>
     </row>
-    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="30" t="s">
         <v>252</v>
       </c>
@@ -9381,7 +9401,7 @@
       </c>
       <c r="I232" s="32"/>
     </row>
-    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="30" t="s">
         <v>253</v>
       </c>
@@ -9406,7 +9426,7 @@
       </c>
       <c r="I233" s="32"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="30" t="s">
         <v>254</v>
       </c>
@@ -9431,7 +9451,7 @@
       </c>
       <c r="I234" s="32"/>
     </row>
-    <row r="235" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="30" t="s">
         <v>255</v>
       </c>
@@ -9456,7 +9476,7 @@
       </c>
       <c r="I235" s="32"/>
     </row>
-    <row r="236" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="30" t="s">
         <v>256</v>
       </c>
@@ -9481,7 +9501,7 @@
       </c>
       <c r="I236" s="32"/>
     </row>
-    <row r="237" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="30" t="s">
         <v>257</v>
       </c>
@@ -9506,7 +9526,7 @@
       </c>
       <c r="I237" s="32"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="30" t="s">
         <v>258</v>
       </c>
@@ -9531,7 +9551,7 @@
       </c>
       <c r="I238" s="32"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="30" t="s">
         <v>259</v>
       </c>
@@ -9556,7 +9576,7 @@
       </c>
       <c r="I239" s="32"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="30" t="s">
         <v>260</v>
       </c>
@@ -9581,7 +9601,7 @@
       </c>
       <c r="I240" s="32"/>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="30" t="s">
         <v>261</v>
       </c>
@@ -9606,7 +9626,7 @@
       </c>
       <c r="I241" s="32"/>
     </row>
-    <row r="242" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="30" t="s">
         <v>262</v>
       </c>
@@ -9883,13 +9903,13 @@
     </row>
     <row r="253" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A253" s="22" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B253" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C253" s="20" t="s">
-        <v>675</v>
+        <v>689</v>
       </c>
       <c r="D253" s="30"/>
       <c r="E253" s="30" t="s">
@@ -9908,63 +9928,63 @@
     </row>
     <row r="254" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A254" s="22" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B254" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C254" s="20" t="s">
-        <v>687</v>
-      </c>
-      <c r="D254" s="47"/>
-      <c r="E254" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F254" s="47" t="s">
+        <v>686</v>
+      </c>
+      <c r="D254" s="34"/>
+      <c r="E254" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F254" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G254" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="H254" s="47" t="s">
+      <c r="G254" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H254" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I254" s="48"/>
+      <c r="I254" s="35"/>
     </row>
     <row r="255" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="22" t="s">
-        <v>684</v>
-      </c>
-      <c r="B255" s="31" t="s">
-        <v>345</v>
+        <v>687</v>
+      </c>
+      <c r="B255" s="24" t="s">
+        <v>688</v>
       </c>
       <c r="C255" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="D255" s="22"/>
+      <c r="E255" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F255" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G255" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H255" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I255" s="20"/>
+    </row>
+    <row r="256" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A256" s="22" t="s">
         <v>683</v>
-      </c>
-      <c r="D255" s="30"/>
-      <c r="E255" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F255" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G255" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H255" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I255" s="32"/>
-    </row>
-    <row r="256" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A256" s="30" t="s">
-        <v>273</v>
       </c>
       <c r="B256" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C256" s="20" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="D256" s="30"/>
       <c r="E256" s="30" t="s">
@@ -9977,44 +9997,44 @@
         <v>15</v>
       </c>
       <c r="H256" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I256" s="32"/>
     </row>
-    <row r="257" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B257" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="C257" s="32" t="s">
-        <v>569</v>
+      <c r="C257" s="20" t="s">
+        <v>675</v>
       </c>
       <c r="D257" s="30"/>
       <c r="E257" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F257" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G257" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H257" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I257" s="32"/>
     </row>
     <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B258" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C258" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D258" s="30"/>
       <c r="E258" s="30" t="s">
@@ -10024,22 +10044,22 @@
         <v>6</v>
       </c>
       <c r="G258" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H258" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I258" s="32"/>
     </row>
     <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B259" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C259" s="32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D259" s="30"/>
       <c r="E259" s="30" t="s">
@@ -10052,19 +10072,19 @@
         <v>15</v>
       </c>
       <c r="H259" s="30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I259" s="32"/>
     </row>
-    <row r="260" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A260" s="22" t="s">
-        <v>277</v>
+    <row r="260" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="30" t="s">
+        <v>276</v>
       </c>
       <c r="B260" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="C260" s="20" t="s">
-        <v>664</v>
+      <c r="C260" s="32" t="s">
+        <v>571</v>
       </c>
       <c r="D260" s="30"/>
       <c r="E260" s="30" t="s">
@@ -10077,21 +10097,19 @@
         <v>15</v>
       </c>
       <c r="H260" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I260" s="20" t="s">
-        <v>668</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I260" s="32"/>
     </row>
     <row r="261" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A261" s="30" t="s">
-        <v>278</v>
+      <c r="A261" s="22" t="s">
+        <v>277</v>
       </c>
       <c r="B261" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="C261" s="32" t="s">
-        <v>572</v>
+      <c r="C261" s="20" t="s">
+        <v>664</v>
       </c>
       <c r="D261" s="30"/>
       <c r="E261" s="30" t="s">
@@ -10104,76 +10122,76 @@
         <v>15</v>
       </c>
       <c r="H261" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I261" s="32"/>
-    </row>
-    <row r="262" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A262" s="22" t="s">
-        <v>279</v>
+        <v>17</v>
+      </c>
+      <c r="I261" s="20" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A262" s="30" t="s">
+        <v>278</v>
       </c>
       <c r="B262" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="C262" s="20" t="s">
-        <v>669</v>
+      <c r="C262" s="32" t="s">
+        <v>572</v>
       </c>
       <c r="D262" s="30"/>
       <c r="E262" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F262" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G262" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H262" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I262" s="20" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A263" s="30" t="s">
-        <v>280</v>
+        <v>20</v>
+      </c>
+      <c r="I262" s="32"/>
+    </row>
+    <row r="263" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A263" s="22" t="s">
+        <v>279</v>
       </c>
       <c r="B263" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="C263" s="32" t="s">
-        <v>573</v>
-      </c>
-      <c r="D263" s="30" t="s">
-        <v>618</v>
-      </c>
+      <c r="C263" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="D263" s="30"/>
       <c r="E263" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F263" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G263" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H263" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I263" s="32"/>
+        <v>17</v>
+      </c>
+      <c r="I263" s="20" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="264" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B264" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C264" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D264" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E264" s="30" t="s">
         <v>19</v>
@@ -10191,16 +10209,16 @@
     </row>
     <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B265" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C265" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D265" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E265" s="30" t="s">
         <v>19</v>
@@ -10216,18 +10234,18 @@
       </c>
       <c r="I265" s="32"/>
     </row>
-    <row r="266" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B266" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C266" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D266" s="30" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E266" s="30" t="s">
         <v>19</v>
@@ -10245,16 +10263,16 @@
     </row>
     <row r="267" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A267" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B267" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C267" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D267" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E267" s="30" t="s">
         <v>19</v>
@@ -10272,16 +10290,16 @@
     </row>
     <row r="268" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A268" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B268" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C268" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D268" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E268" s="30" t="s">
         <v>19</v>
@@ -10297,40 +10315,42 @@
       </c>
       <c r="I268" s="32"/>
     </row>
-    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A269" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="B269" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="C269" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="D269" s="30" t="s">
+        <v>623</v>
+      </c>
+      <c r="E269" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F269" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G269" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H269" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I269" s="32"/>
+    </row>
+    <row r="270" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="30" t="s">
         <v>286</v>
-      </c>
-      <c r="B269" s="31" t="s">
-        <v>346</v>
-      </c>
-      <c r="C269" s="32" t="s">
-        <v>579</v>
-      </c>
-      <c r="D269" s="30"/>
-      <c r="E269" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F269" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G269" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H269" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I269" s="32"/>
-    </row>
-    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A270" s="30" t="s">
-        <v>287</v>
       </c>
       <c r="B270" s="31" t="s">
         <v>346</v>
       </c>
       <c r="C270" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D270" s="30"/>
       <c r="E270" s="30" t="s">
@@ -10340,22 +10360,22 @@
         <v>7</v>
       </c>
       <c r="G270" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H270" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I270" s="32"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B271" s="31" t="s">
         <v>346</v>
       </c>
       <c r="C271" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D271" s="30"/>
       <c r="E271" s="30" t="s">
@@ -10372,40 +10392,40 @@
       </c>
       <c r="I271" s="32"/>
     </row>
-    <row r="272" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B272" s="31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C272" s="32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D272" s="30"/>
       <c r="E272" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F272" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G272" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H272" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I272" s="32"/>
     </row>
-    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B273" s="31" t="s">
         <v>347</v>
       </c>
       <c r="C273" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D273" s="30"/>
       <c r="E273" s="30" t="s">
@@ -10422,40 +10442,40 @@
       </c>
       <c r="I273" s="32"/>
     </row>
-    <row r="274" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B274" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C274" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D274" s="30"/>
       <c r="E274" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F274" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G274" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H274" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I274" s="32"/>
     </row>
-    <row r="275" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B275" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C275" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D275" s="30"/>
       <c r="E275" s="30" t="s">
@@ -10472,15 +10492,15 @@
       </c>
       <c r="I275" s="32"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B276" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C276" s="32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D276" s="30"/>
       <c r="E276" s="30" t="s">
@@ -10490,22 +10510,22 @@
         <v>7</v>
       </c>
       <c r="G276" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H276" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I276" s="32"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B277" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C277" s="32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D277" s="30"/>
       <c r="E277" s="30" t="s">
@@ -10515,22 +10535,22 @@
         <v>7</v>
       </c>
       <c r="G277" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H277" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I277" s="32"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B278" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C278" s="32" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D278" s="30"/>
       <c r="E278" s="30" t="s">
@@ -10547,15 +10567,15 @@
       </c>
       <c r="I278" s="32"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B279" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C279" s="32" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D279" s="30"/>
       <c r="E279" s="30" t="s">
@@ -10572,40 +10592,40 @@
       </c>
       <c r="I279" s="32"/>
     </row>
-    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B280" s="31" t="s">
         <v>348</v>
       </c>
       <c r="C280" s="32" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D280" s="30"/>
       <c r="E280" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F280" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G280" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H280" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I280" s="32"/>
     </row>
-    <row r="281" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B281" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C281" s="32" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D281" s="30"/>
       <c r="E281" s="30" t="s">
@@ -10615,47 +10635,47 @@
         <v>3</v>
       </c>
       <c r="G281" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H281" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I281" s="32"/>
     </row>
-    <row r="282" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B282" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C282" s="32" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D282" s="30"/>
       <c r="E282" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F282" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G282" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H282" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I282" s="32"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B283" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C283" s="32" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D283" s="30"/>
       <c r="E283" s="30" t="s">
@@ -10672,65 +10692,65 @@
       </c>
       <c r="I283" s="32"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B284" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C284" s="32" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D284" s="30"/>
       <c r="E284" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F284" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G284" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H284" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I284" s="32"/>
     </row>
-    <row r="285" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B285" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C285" s="32" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D285" s="30"/>
       <c r="E285" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F285" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G285" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H285" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I285" s="32"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B286" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C286" s="32" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D286" s="30"/>
       <c r="E286" s="30" t="s">
@@ -10740,22 +10760,22 @@
         <v>6</v>
       </c>
       <c r="G286" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H286" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I286" s="32"/>
     </row>
-    <row r="287" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B287" s="31" t="s">
         <v>349</v>
       </c>
       <c r="C287" s="32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D287" s="30"/>
       <c r="E287" s="30" t="s">
@@ -10765,83 +10785,79 @@
         <v>6</v>
       </c>
       <c r="G287" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H287" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I287" s="32"/>
+    </row>
+    <row r="288" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="30" t="s">
+        <v>304</v>
+      </c>
+      <c r="B288" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="C288" s="32" t="s">
+        <v>597</v>
+      </c>
+      <c r="D288" s="30"/>
+      <c r="E288" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F288" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G288" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H288" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="I287" s="32"/>
-    </row>
-    <row r="288" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A288" s="30" t="s">
+      <c r="I288" s="32"/>
+    </row>
+    <row r="289" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="30" t="s">
         <v>305</v>
-      </c>
-      <c r="B288" s="31" t="s">
-        <v>350</v>
-      </c>
-      <c r="C288" s="32" t="s">
-        <v>598</v>
-      </c>
-      <c r="D288" s="30" t="s">
-        <v>624</v>
-      </c>
-      <c r="E288" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F288" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G288" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H288" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I288" s="32" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="289" spans="1:9" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A289" s="22" t="s">
-        <v>306</v>
       </c>
       <c r="B289" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C289" s="32" t="s">
-        <v>599</v>
-      </c>
-      <c r="D289" s="22" t="s">
-        <v>679</v>
+        <v>598</v>
+      </c>
+      <c r="D289" s="30" t="s">
+        <v>624</v>
       </c>
       <c r="E289" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F289" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G289" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H289" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I289" s="32" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="290" spans="1:9" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A290" s="30" t="s">
-        <v>307</v>
+    <row r="290" spans="1:9" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="22" t="s">
+        <v>306</v>
       </c>
       <c r="B290" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="C290" s="20" t="s">
-        <v>600</v>
+      <c r="C290" s="32" t="s">
+        <v>599</v>
       </c>
       <c r="D290" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E290" s="30" t="s">
         <v>22</v>
@@ -10859,18 +10875,18 @@
         <v>635</v>
       </c>
     </row>
-    <row r="291" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B291" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C291" s="20" t="s">
-        <v>670</v>
+        <v>600</v>
       </c>
       <c r="D291" s="22" t="s">
-        <v>625</v>
+        <v>678</v>
       </c>
       <c r="E291" s="30" t="s">
         <v>22</v>
@@ -10888,17 +10904,17 @@
         <v>635</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B292" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C292" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="D292" s="30" t="s">
+        <v>670</v>
+      </c>
+      <c r="D292" s="22" t="s">
         <v>625</v>
       </c>
       <c r="E292" s="30" t="s">
@@ -10917,24 +10933,24 @@
         <v>635</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B293" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="C293" s="32" t="s">
-        <v>601</v>
-      </c>
-      <c r="D293" s="22" t="s">
-        <v>626</v>
+      <c r="C293" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="D293" s="30" t="s">
+        <v>625</v>
       </c>
       <c r="E293" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F293" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G293" s="30" t="s">
         <v>15</v>
@@ -10946,17 +10962,17 @@
         <v>635</v>
       </c>
     </row>
-    <row r="294" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B294" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="C294" s="20" t="s">
-        <v>602</v>
-      </c>
-      <c r="D294" s="30" t="s">
+      <c r="C294" s="32" t="s">
+        <v>601</v>
+      </c>
+      <c r="D294" s="22" t="s">
         <v>626</v>
       </c>
       <c r="E294" s="30" t="s">
@@ -10975,15 +10991,15 @@
         <v>635</v>
       </c>
     </row>
-    <row r="295" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B295" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C295" s="20" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D295" s="30" t="s">
         <v>626</v>
@@ -11004,18 +11020,18 @@
         <v>635</v>
       </c>
     </row>
-    <row r="296" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A296" s="22" t="s">
-        <v>649</v>
-      </c>
-      <c r="B296" s="24" t="s">
+    <row r="296" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="B296" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C296" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="D296" s="22" t="s">
-        <v>648</v>
+        <v>603</v>
+      </c>
+      <c r="D296" s="30" t="s">
+        <v>626</v>
       </c>
       <c r="E296" s="30" t="s">
         <v>22</v>
@@ -11027,22 +11043,24 @@
         <v>15</v>
       </c>
       <c r="H296" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I296" s="32"/>
-    </row>
-    <row r="297" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I296" s="32" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="22" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B297" s="24" t="s">
         <v>350</v>
       </c>
       <c r="C297" s="20" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D297" s="22" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E297" s="30" t="s">
         <v>22</v>
@@ -11058,46 +11076,44 @@
       </c>
       <c r="I297" s="32"/>
     </row>
-    <row r="298" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A298" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="B298" s="31" t="s">
+    <row r="298" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="B298" s="24" t="s">
         <v>350</v>
       </c>
       <c r="C298" s="20" t="s">
-        <v>672</v>
+        <v>652</v>
       </c>
       <c r="D298" s="22" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="E298" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F298" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G298" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H298" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I298" s="32" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="299" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="I298" s="32"/>
+    </row>
+    <row r="299" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B299" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C299" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="D299" s="30" t="s">
+        <v>672</v>
+      </c>
+      <c r="D299" s="22" t="s">
         <v>627</v>
       </c>
       <c r="E299" s="30" t="s">
@@ -11116,18 +11132,18 @@
         <v>635</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A300" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="B300" s="24" t="s">
+    <row r="300" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="B300" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C300" s="20" t="s">
-        <v>659</v>
-      </c>
-      <c r="D300" s="22" t="s">
-        <v>657</v>
+        <v>673</v>
+      </c>
+      <c r="D300" s="30" t="s">
+        <v>627</v>
       </c>
       <c r="E300" s="30" t="s">
         <v>22</v>
@@ -11139,19 +11155,21 @@
         <v>15</v>
       </c>
       <c r="H300" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I300" s="32"/>
-    </row>
-    <row r="301" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I300" s="32" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="22" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B301" s="24" t="s">
         <v>350</v>
       </c>
       <c r="C301" s="20" t="s">
-        <v>677</v>
+        <v>659</v>
       </c>
       <c r="D301" s="22" t="s">
         <v>657</v>
@@ -11166,24 +11184,22 @@
         <v>15</v>
       </c>
       <c r="H301" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I301" s="32" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="302" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="I301" s="32"/>
+    </row>
+    <row r="302" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="22" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="B302" s="24" t="s">
         <v>350</v>
       </c>
       <c r="C302" s="20" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
       <c r="D302" s="22" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="E302" s="30" t="s">
         <v>22</v>
@@ -11201,40 +11217,44 @@
         <v>635</v>
       </c>
     </row>
-    <row r="303" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="B303" s="31" t="s">
+        <v>666</v>
+      </c>
+      <c r="B303" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="C303" s="32" t="s">
-        <v>604</v>
-      </c>
-      <c r="D303" s="30"/>
+      <c r="C303" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="D303" s="22" t="s">
+        <v>665</v>
+      </c>
       <c r="E303" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F303" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G303" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H303" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I303" s="32"/>
-    </row>
-    <row r="304" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A304" s="30" t="s">
-        <v>316</v>
+        <v>20</v>
+      </c>
+      <c r="I303" s="32" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="22" t="s">
+        <v>315</v>
       </c>
       <c r="B304" s="31" t="s">
         <v>350</v>
       </c>
       <c r="C304" s="32" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D304" s="30"/>
       <c r="E304" s="30" t="s">
@@ -11251,13 +11271,38 @@
       </c>
       <c r="I304" s="32"/>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="3"/>
-      <c r="B305" s="10"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="B305" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="C305" s="32" t="s">
+        <v>605</v>
+      </c>
+      <c r="D305" s="30"/>
+      <c r="E305" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F305" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G305" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H305" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I305" s="32"/>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" s="3"/>
       <c r="B306" s="10"/>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A307" s="3"/>
+      <c r="B307" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -11275,51 +11320,51 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:I304">
-    <cfRule type="expression" dxfId="7" priority="53">
+  <conditionalFormatting sqref="A20:I305">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:I304">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <conditionalFormatting sqref="A20:I305">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F304">
-    <cfRule type="expression" dxfId="1" priority="13">
+  <conditionalFormatting sqref="F20:F305">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F304" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F305" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E304" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E305" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G304" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G305" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H304" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H305" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11329,7 +11374,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B255:B306 B19:B253" numberStoredAsText="1"/>
+    <ignoredError sqref="B256:B307 B19:B253" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Updated md and RS and config files of MS-COPYS.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-COPYS/MS-COPYS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2082920-71AE-40D6-A5D1-B2A3129758B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC615A95-8A38-4882-8B4B-FC7FEFAAE2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2085" windowWidth="24240" windowHeight="13290" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -2398,9 +2398,6 @@
     <t>Verified by derived requirement: MS-COPYS_R2781.</t>
   </si>
   <si>
-    <t>[In CopyIntoItemsLocal] Unless otherwise specified, the method behavior for the source IRI, content, fields, and destination locations for the CopyItemsIntoLocal operation is the same as the CopyIntoItems operation, as specified in section 3.1.4.2.&lt;6&gt;</t>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior] [For CopyIntoItems operation] Implementation [the value of field with internal name _CopySource ] does equal to the value of source location.(Windows SharePoint Services 3.0, SharePoint Foundation 2010 and SharePoint Foundation 2013 follow this behavior.)</t>
   </si>
   <si>
@@ -2473,6 +2470,9 @@
   <si>
     <t>[In CopyIntoItemsLocal] If the source location does not point to an existing file, then if the destination location points to an existing file whose permission setting does not allow access by the protocol client, the protocol server MUST report a failure by returning the CopyResult element with the ErrorCode attribute set to "Unknown" for this destination location.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In CopyIntoItemsLocal] Unless otherwise specified, the method behavior for the source IRI, content, fields, and destination locations for the CopyIntoItemsLocal operation is the same as the CopyIntoItems operation, as specified in section 3.1.4.2.&lt;6&gt;</t>
   </si>
 </sst>
 </file>
@@ -2480,14 +2480,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2690,13 +2690,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2729,7 +2729,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3690,24 +3690,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L307"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>636</v>
       </c>
@@ -3717,7 +3719,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
         <v>637</v>
       </c>
@@ -3728,22 +3730,22 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>638</v>
       </c>
       <c r="F3" s="12">
-        <v>43634</v>
+        <v>44474</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21">
       <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
@@ -3755,7 +3757,7 @@
       <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
@@ -3771,7 +3773,7 @@
       <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -3787,7 +3789,7 @@
       <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -3803,7 +3805,7 @@
       <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -3819,7 +3821,7 @@
       <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
@@ -3835,7 +3837,7 @@
       <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -3851,7 +3853,7 @@
       <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -3867,7 +3869,7 @@
       <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -3885,7 +3887,7 @@
       <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -3903,7 +3905,7 @@
       <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -3921,7 +3923,7 @@
       <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -3939,7 +3941,7 @@
       <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
@@ -3955,7 +3957,7 @@
       <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3971,7 +3973,7 @@
       <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3988,7 +3990,7 @@
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -4018,7 +4020,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="23" customFormat="1" hidden="1">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
@@ -4043,7 +4045,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -4070,7 +4072,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -4095,7 +4097,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A23" s="22" t="s">
         <v>46</v>
       </c>
@@ -4103,7 +4105,7 @@
         <v>317</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -4120,7 +4122,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A24" s="22" t="s">
         <v>47</v>
       </c>
@@ -4145,7 +4147,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
@@ -4153,7 +4155,7 @@
         <v>317</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -4170,7 +4172,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -4195,7 +4197,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="45" hidden="1">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -4220,7 +4222,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -4245,7 +4247,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="45" hidden="1">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
@@ -4270,7 +4272,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A30" s="22" t="s">
         <v>53</v>
       </c>
@@ -4295,7 +4297,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -4320,7 +4322,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="23" customFormat="1" hidden="1">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -4345,7 +4347,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="30" hidden="1">
       <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
@@ -4370,7 +4372,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" hidden="1">
       <c r="A34" s="30" t="s">
         <v>57</v>
       </c>
@@ -4395,7 +4397,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" hidden="1">
       <c r="A35" s="30" t="s">
         <v>58</v>
       </c>
@@ -4420,7 +4422,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" hidden="1">
       <c r="A36" s="30" t="s">
         <v>59</v>
       </c>
@@ -4445,7 +4447,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" hidden="1">
       <c r="A37" s="30" t="s">
         <v>60</v>
       </c>
@@ -4470,7 +4472,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" hidden="1">
       <c r="A38" s="30" t="s">
         <v>61</v>
       </c>
@@ -4495,7 +4497,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" hidden="1">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>
@@ -4520,7 +4522,7 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="165" hidden="1">
       <c r="A40" s="30" t="s">
         <v>63</v>
       </c>
@@ -4545,7 +4547,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1">
       <c r="A41" s="30" t="s">
         <v>64</v>
       </c>
@@ -4570,7 +4572,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="45" hidden="1">
       <c r="A42" s="30" t="s">
         <v>65</v>
       </c>
@@ -4595,7 +4597,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" hidden="1">
       <c r="A43" s="30" t="s">
         <v>66</v>
       </c>
@@ -4620,7 +4622,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" hidden="1">
       <c r="A44" s="30" t="s">
         <v>67</v>
       </c>
@@ -4645,7 +4647,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" hidden="1">
       <c r="A45" s="30" t="s">
         <v>68</v>
       </c>
@@ -4670,7 +4672,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30" hidden="1">
       <c r="A46" s="30" t="s">
         <v>69</v>
       </c>
@@ -4695,7 +4697,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="45" hidden="1">
       <c r="A47" s="30" t="s">
         <v>70</v>
       </c>
@@ -4720,7 +4722,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" hidden="1">
       <c r="A48" s="30" t="s">
         <v>71</v>
       </c>
@@ -4745,7 +4747,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" hidden="1">
       <c r="A49" s="30" t="s">
         <v>72</v>
       </c>
@@ -4770,7 +4772,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30" hidden="1">
       <c r="A50" s="30" t="s">
         <v>73</v>
       </c>
@@ -4795,7 +4797,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30" hidden="1">
       <c r="A51" s="30" t="s">
         <v>74</v>
       </c>
@@ -4820,7 +4822,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="105" hidden="1">
       <c r="A52" s="30" t="s">
         <v>75</v>
       </c>
@@ -4845,7 +4847,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" s="30" t="s">
         <v>76</v>
       </c>
@@ -4870,7 +4872,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" s="30" t="s">
         <v>77</v>
       </c>
@@ -4895,7 +4897,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" hidden="1">
       <c r="A55" s="30" t="s">
         <v>78</v>
       </c>
@@ -4920,7 +4922,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="90" hidden="1">
       <c r="A56" s="30" t="s">
         <v>79</v>
       </c>
@@ -4945,7 +4947,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="30" hidden="1">
       <c r="A57" s="30" t="s">
         <v>80</v>
       </c>
@@ -4970,7 +4972,7 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30" hidden="1">
       <c r="A58" s="30" t="s">
         <v>81</v>
       </c>
@@ -4995,7 +4997,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30" hidden="1">
       <c r="A59" s="30" t="s">
         <v>82</v>
       </c>
@@ -5020,7 +5022,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" hidden="1">
       <c r="A60" s="30" t="s">
         <v>83</v>
       </c>
@@ -5047,7 +5049,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" hidden="1">
       <c r="A61" s="30" t="s">
         <v>84</v>
       </c>
@@ -5074,7 +5076,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="45" hidden="1">
       <c r="A62" s="30" t="s">
         <v>85</v>
       </c>
@@ -5099,7 +5101,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="45" hidden="1">
       <c r="A63" s="30" t="s">
         <v>86</v>
       </c>
@@ -5126,7 +5128,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="45" hidden="1">
       <c r="A64" s="30" t="s">
         <v>87</v>
       </c>
@@ -5153,7 +5155,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" hidden="1">
       <c r="A65" s="30" t="s">
         <v>88</v>
       </c>
@@ -5178,7 +5180,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" hidden="1">
       <c r="A66" s="30" t="s">
         <v>89</v>
       </c>
@@ -5203,7 +5205,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30" hidden="1">
       <c r="A67" s="30" t="s">
         <v>90</v>
       </c>
@@ -5228,7 +5230,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="105" hidden="1">
       <c r="A68" s="30" t="s">
         <v>91</v>
       </c>
@@ -5253,7 +5255,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30" hidden="1">
       <c r="A69" s="30" t="s">
         <v>92</v>
       </c>
@@ -5278,7 +5280,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30" hidden="1">
       <c r="A70" s="30" t="s">
         <v>93</v>
       </c>
@@ -5303,7 +5305,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1">
       <c r="A71" s="30" t="s">
         <v>94</v>
       </c>
@@ -5328,7 +5330,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="120" hidden="1">
       <c r="A72" s="30" t="s">
         <v>95</v>
       </c>
@@ -5353,7 +5355,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1">
       <c r="A73" s="30" t="s">
         <v>96</v>
       </c>
@@ -5378,7 +5380,7 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="60" hidden="1">
       <c r="A74" s="30" t="s">
         <v>97</v>
       </c>
@@ -5403,7 +5405,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1">
       <c r="A75" s="30" t="s">
         <v>98</v>
       </c>
@@ -5428,7 +5430,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" hidden="1">
       <c r="A76" s="30" t="s">
         <v>99</v>
       </c>
@@ -5453,7 +5455,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" hidden="1">
       <c r="A77" s="30" t="s">
         <v>100</v>
       </c>
@@ -5478,7 +5480,7 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="30" hidden="1">
       <c r="A78" s="30" t="s">
         <v>101</v>
       </c>
@@ -5503,7 +5505,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30" hidden="1">
       <c r="A79" s="30" t="s">
         <v>102</v>
       </c>
@@ -5528,7 +5530,7 @@
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1">
       <c r="A80" s="30" t="s">
         <v>103</v>
       </c>
@@ -5553,7 +5555,7 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30" hidden="1">
       <c r="A81" s="30" t="s">
         <v>104</v>
       </c>
@@ -5578,7 +5580,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="30" hidden="1">
       <c r="A82" s="30" t="s">
         <v>105</v>
       </c>
@@ -5605,7 +5607,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" hidden="1">
       <c r="A83" s="30" t="s">
         <v>106</v>
       </c>
@@ -5632,7 +5634,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30" hidden="1">
       <c r="A84" s="30" t="s">
         <v>107</v>
       </c>
@@ -5659,7 +5661,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30" hidden="1">
       <c r="A85" s="30" t="s">
         <v>108</v>
       </c>
@@ -5686,7 +5688,7 @@
       </c>
       <c r="I85" s="32"/>
     </row>
-    <row r="86" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="105" hidden="1">
       <c r="A86" s="30" t="s">
         <v>109</v>
       </c>
@@ -5711,7 +5713,7 @@
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" hidden="1">
       <c r="A87" s="30" t="s">
         <v>110</v>
       </c>
@@ -5736,7 +5738,7 @@
       </c>
       <c r="I87" s="32"/>
     </row>
-    <row r="88" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" hidden="1">
       <c r="A88" s="30" t="s">
         <v>111</v>
       </c>
@@ -5761,7 +5763,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30" hidden="1">
       <c r="A89" s="30" t="s">
         <v>112</v>
       </c>
@@ -5786,7 +5788,7 @@
       </c>
       <c r="I89" s="32"/>
     </row>
-    <row r="90" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30" hidden="1">
       <c r="A90" s="30" t="s">
         <v>113</v>
       </c>
@@ -5811,7 +5813,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30" hidden="1">
       <c r="A91" s="30" t="s">
         <v>114</v>
       </c>
@@ -5836,7 +5838,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30" hidden="1">
       <c r="A92" s="30" t="s">
         <v>115</v>
       </c>
@@ -5861,7 +5863,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="30" hidden="1">
       <c r="A93" s="30" t="s">
         <v>116</v>
       </c>
@@ -5886,7 +5888,7 @@
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="180" hidden="1">
       <c r="A94" s="30" t="s">
         <v>117</v>
       </c>
@@ -5911,7 +5913,7 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="45" hidden="1">
       <c r="A95" s="30" t="s">
         <v>118</v>
       </c>
@@ -5936,7 +5938,7 @@
       </c>
       <c r="I95" s="32"/>
     </row>
-    <row r="96" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="30" hidden="1">
       <c r="A96" s="30" t="s">
         <v>119</v>
       </c>
@@ -5961,7 +5963,7 @@
       </c>
       <c r="I96" s="32"/>
     </row>
-    <row r="97" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30" hidden="1">
       <c r="A97" s="30" t="s">
         <v>120</v>
       </c>
@@ -5988,7 +5990,7 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="30" hidden="1">
       <c r="A98" s="30" t="s">
         <v>121</v>
       </c>
@@ -6015,7 +6017,7 @@
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30" hidden="1">
       <c r="A99" s="30" t="s">
         <v>122</v>
       </c>
@@ -6040,7 +6042,7 @@
       </c>
       <c r="I99" s="32"/>
     </row>
-    <row r="100" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30" hidden="1">
       <c r="A100" s="30" t="s">
         <v>123</v>
       </c>
@@ -6065,7 +6067,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="45" hidden="1">
       <c r="A101" s="30" t="s">
         <v>124</v>
       </c>
@@ -6090,7 +6092,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="45" hidden="1">
       <c r="A102" s="30" t="s">
         <v>125</v>
       </c>
@@ -6117,7 +6119,7 @@
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="45" hidden="1">
       <c r="A103" s="30" t="s">
         <v>126</v>
       </c>
@@ -6144,7 +6146,7 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30" hidden="1">
       <c r="A104" s="30" t="s">
         <v>127</v>
       </c>
@@ -6169,7 +6171,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="45" hidden="1">
       <c r="A105" s="30" t="s">
         <v>128</v>
       </c>
@@ -6194,7 +6196,7 @@
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="45" hidden="1">
       <c r="A106" s="30" t="s">
         <v>129</v>
       </c>
@@ -6221,7 +6223,7 @@
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="45" hidden="1">
       <c r="A107" s="30" t="s">
         <v>130</v>
       </c>
@@ -6248,7 +6250,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30" hidden="1">
       <c r="A108" s="22" t="s">
         <v>131</v>
       </c>
@@ -6273,7 +6275,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="45" hidden="1">
       <c r="A109" s="30" t="s">
         <v>132</v>
       </c>
@@ -6298,7 +6300,7 @@
       </c>
       <c r="I109" s="32"/>
     </row>
-    <row r="110" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="45" hidden="1">
       <c r="A110" s="30" t="s">
         <v>133</v>
       </c>
@@ -6325,7 +6327,7 @@
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30" hidden="1">
       <c r="A111" s="30" t="s">
         <v>134</v>
       </c>
@@ -6352,7 +6354,7 @@
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="30" hidden="1">
       <c r="A112" s="30" t="s">
         <v>135</v>
       </c>
@@ -6377,7 +6379,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="409.5" hidden="1">
       <c r="A113" s="30" t="s">
         <v>136</v>
       </c>
@@ -6402,7 +6404,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="75" hidden="1">
       <c r="A114" s="30" t="s">
         <v>137</v>
       </c>
@@ -6427,7 +6429,7 @@
       </c>
       <c r="I114" s="32"/>
     </row>
-    <row r="115" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="60" hidden="1">
       <c r="A115" s="30" t="s">
         <v>138</v>
       </c>
@@ -6454,7 +6456,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1">
       <c r="A116" s="30" t="s">
         <v>139</v>
       </c>
@@ -6481,7 +6483,7 @@
       </c>
       <c r="I116" s="32"/>
     </row>
-    <row r="117" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="60" hidden="1">
       <c r="A117" s="22" t="s">
         <v>140</v>
       </c>
@@ -6508,7 +6510,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1">
       <c r="A118" s="22" t="s">
         <v>644</v>
       </c>
@@ -6533,7 +6535,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1">
       <c r="A119" s="22" t="s">
         <v>646</v>
       </c>
@@ -6558,7 +6560,7 @@
       </c>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="60" hidden="1">
       <c r="A120" s="30" t="s">
         <v>141</v>
       </c>
@@ -6583,7 +6585,7 @@
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="30" hidden="1">
       <c r="A121" s="30" t="s">
         <v>142</v>
       </c>
@@ -6608,7 +6610,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="90" hidden="1">
       <c r="A122" s="30" t="s">
         <v>143</v>
       </c>
@@ -6633,7 +6635,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1">
       <c r="A123" s="30" t="s">
         <v>144</v>
       </c>
@@ -6658,7 +6660,7 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1">
       <c r="A124" s="30" t="s">
         <v>145</v>
       </c>
@@ -6683,7 +6685,7 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="30" hidden="1">
       <c r="A125" s="30" t="s">
         <v>146</v>
       </c>
@@ -6708,7 +6710,7 @@
       </c>
       <c r="I125" s="32"/>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1">
       <c r="A126" s="30" t="s">
         <v>147</v>
       </c>
@@ -6733,7 +6735,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="30" hidden="1">
       <c r="A127" s="30" t="s">
         <v>148</v>
       </c>
@@ -6758,7 +6760,7 @@
       </c>
       <c r="I127" s="32"/>
     </row>
-    <row r="128" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="45" hidden="1">
       <c r="A128" s="30" t="s">
         <v>149</v>
       </c>
@@ -6783,7 +6785,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="30" hidden="1">
       <c r="A129" s="30" t="s">
         <v>150</v>
       </c>
@@ -6808,7 +6810,7 @@
       </c>
       <c r="I129" s="32"/>
     </row>
-    <row r="130" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="30" hidden="1">
       <c r="A130" s="30" t="s">
         <v>151</v>
       </c>
@@ -6833,7 +6835,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="45" hidden="1">
       <c r="A131" s="30" t="s">
         <v>152</v>
       </c>
@@ -6858,7 +6860,7 @@
       </c>
       <c r="I131" s="32"/>
     </row>
-    <row r="132" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30" hidden="1">
       <c r="A132" s="30" t="s">
         <v>153</v>
       </c>
@@ -6883,7 +6885,7 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1">
       <c r="A133" s="30" t="s">
         <v>154</v>
       </c>
@@ -6908,7 +6910,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1">
       <c r="A134" s="30" t="s">
         <v>155</v>
       </c>
@@ -6933,7 +6935,7 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30" hidden="1">
       <c r="A135" s="30" t="s">
         <v>156</v>
       </c>
@@ -6958,7 +6960,7 @@
       </c>
       <c r="I135" s="32"/>
     </row>
-    <row r="136" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="30" hidden="1">
       <c r="A136" s="30" t="s">
         <v>157</v>
       </c>
@@ -6983,7 +6985,7 @@
       </c>
       <c r="I136" s="32"/>
     </row>
-    <row r="137" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="45" hidden="1">
       <c r="A137" s="30" t="s">
         <v>158</v>
       </c>
@@ -7008,7 +7010,7 @@
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="45" hidden="1">
       <c r="A138" s="30" t="s">
         <v>159</v>
       </c>
@@ -7033,7 +7035,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="45" hidden="1">
       <c r="A139" s="30" t="s">
         <v>160</v>
       </c>
@@ -7060,7 +7062,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="30" hidden="1">
       <c r="A140" s="30" t="s">
         <v>161</v>
       </c>
@@ -7085,7 +7087,7 @@
       </c>
       <c r="I140" s="32"/>
     </row>
-    <row r="141" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="45" hidden="1">
       <c r="A141" s="30" t="s">
         <v>162</v>
       </c>
@@ -7110,7 +7112,7 @@
       </c>
       <c r="I141" s="32"/>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="30" hidden="1">
       <c r="A142" s="30" t="s">
         <v>163</v>
       </c>
@@ -7135,7 +7137,7 @@
       </c>
       <c r="I142" s="32"/>
     </row>
-    <row r="143" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="30" hidden="1">
       <c r="A143" s="30" t="s">
         <v>164</v>
       </c>
@@ -7160,7 +7162,7 @@
       </c>
       <c r="I143" s="32"/>
     </row>
-    <row r="144" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="30" hidden="1">
       <c r="A144" s="30" t="s">
         <v>165</v>
       </c>
@@ -7187,7 +7189,7 @@
       </c>
       <c r="I144" s="32"/>
     </row>
-    <row r="145" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="45" hidden="1">
       <c r="A145" s="30" t="s">
         <v>166</v>
       </c>
@@ -7214,7 +7216,7 @@
       </c>
       <c r="I145" s="32"/>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" ht="30" hidden="1">
       <c r="A146" s="30" t="s">
         <v>167</v>
       </c>
@@ -7239,7 +7241,7 @@
       </c>
       <c r="I146" s="32"/>
     </row>
-    <row r="147" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" ht="45" hidden="1">
       <c r="A147" s="30" t="s">
         <v>168</v>
       </c>
@@ -7264,7 +7266,7 @@
       </c>
       <c r="I147" s="32"/>
     </row>
-    <row r="148" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="45" hidden="1">
       <c r="A148" s="30" t="s">
         <v>169</v>
       </c>
@@ -7291,7 +7293,7 @@
       </c>
       <c r="I148" s="32"/>
     </row>
-    <row r="149" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="45" hidden="1">
       <c r="A149" s="30" t="s">
         <v>170</v>
       </c>
@@ -7318,7 +7320,7 @@
       </c>
       <c r="I149" s="32"/>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1">
       <c r="A150" s="30" t="s">
         <v>171</v>
       </c>
@@ -7343,7 +7345,7 @@
       </c>
       <c r="I150" s="32"/>
     </row>
-    <row r="151" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="30" hidden="1">
       <c r="A151" s="30" t="s">
         <v>172</v>
       </c>
@@ -7370,7 +7372,7 @@
       </c>
       <c r="I151" s="32"/>
     </row>
-    <row r="152" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="30" hidden="1">
       <c r="A152" s="30" t="s">
         <v>173</v>
       </c>
@@ -7397,7 +7399,7 @@
       </c>
       <c r="I152" s="32"/>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1">
       <c r="A153" s="30" t="s">
         <v>174</v>
       </c>
@@ -7422,7 +7424,7 @@
       </c>
       <c r="I153" s="32"/>
     </row>
-    <row r="154" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="30" hidden="1">
       <c r="A154" s="30" t="s">
         <v>175</v>
       </c>
@@ -7447,7 +7449,7 @@
       </c>
       <c r="I154" s="32"/>
     </row>
-    <row r="155" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="30" hidden="1">
       <c r="A155" s="30" t="s">
         <v>176</v>
       </c>
@@ -7472,7 +7474,7 @@
       </c>
       <c r="I155" s="32"/>
     </row>
-    <row r="156" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="30" hidden="1">
       <c r="A156" s="30" t="s">
         <v>177</v>
       </c>
@@ -7497,7 +7499,7 @@
       </c>
       <c r="I156" s="32"/>
     </row>
-    <row r="157" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="30" hidden="1">
       <c r="A157" s="30" t="s">
         <v>178</v>
       </c>
@@ -7522,7 +7524,7 @@
       </c>
       <c r="I157" s="32"/>
     </row>
-    <row r="158" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="30" hidden="1">
       <c r="A158" s="30" t="s">
         <v>179</v>
       </c>
@@ -7547,7 +7549,7 @@
       </c>
       <c r="I158" s="32"/>
     </row>
-    <row r="159" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="60" hidden="1">
       <c r="A159" s="30" t="s">
         <v>180</v>
       </c>
@@ -7572,7 +7574,7 @@
       </c>
       <c r="I159" s="32"/>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="30" hidden="1">
       <c r="A160" s="30" t="s">
         <v>181</v>
       </c>
@@ -7597,7 +7599,7 @@
       </c>
       <c r="I160" s="32"/>
     </row>
-    <row r="161" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="45" hidden="1">
       <c r="A161" s="30" t="s">
         <v>182</v>
       </c>
@@ -7622,7 +7624,7 @@
       </c>
       <c r="I161" s="32"/>
     </row>
-    <row r="162" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="30" hidden="1">
       <c r="A162" s="30" t="s">
         <v>183</v>
       </c>
@@ -7647,7 +7649,7 @@
       </c>
       <c r="I162" s="32"/>
     </row>
-    <row r="163" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="30" hidden="1">
       <c r="A163" s="30" t="s">
         <v>184</v>
       </c>
@@ -7672,7 +7674,7 @@
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1">
       <c r="A164" s="30" t="s">
         <v>185</v>
       </c>
@@ -7697,7 +7699,7 @@
       </c>
       <c r="I164" s="32"/>
     </row>
-    <row r="165" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="45" hidden="1">
       <c r="A165" s="22" t="s">
         <v>654</v>
       </c>
@@ -7721,10 +7723,10 @@
         <v>17</v>
       </c>
       <c r="I165" s="20" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="45" hidden="1">
       <c r="A166" s="30" t="s">
         <v>186</v>
       </c>
@@ -7749,7 +7751,7 @@
       </c>
       <c r="I166" s="32"/>
     </row>
-    <row r="167" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" ht="60" hidden="1">
       <c r="A167" s="30" t="s">
         <v>187</v>
       </c>
@@ -7774,7 +7776,7 @@
       </c>
       <c r="I167" s="32"/>
     </row>
-    <row r="168" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="60" hidden="1">
       <c r="A168" s="30" t="s">
         <v>188</v>
       </c>
@@ -7799,7 +7801,7 @@
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" ht="60" hidden="1">
       <c r="A169" s="30" t="s">
         <v>189</v>
       </c>
@@ -7824,7 +7826,7 @@
       </c>
       <c r="I169" s="32"/>
     </row>
-    <row r="170" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="30" hidden="1">
       <c r="A170" s="30" t="s">
         <v>190</v>
       </c>
@@ -7849,7 +7851,7 @@
       </c>
       <c r="I170" s="32"/>
     </row>
-    <row r="171" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="30" hidden="1">
       <c r="A171" s="30" t="s">
         <v>191</v>
       </c>
@@ -7874,7 +7876,7 @@
       </c>
       <c r="I171" s="32"/>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1">
       <c r="A172" s="30" t="s">
         <v>192</v>
       </c>
@@ -7899,7 +7901,7 @@
       </c>
       <c r="I172" s="32"/>
     </row>
-    <row r="173" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="30" hidden="1">
       <c r="A173" s="30" t="s">
         <v>193</v>
       </c>
@@ -7924,7 +7926,7 @@
       </c>
       <c r="I173" s="32"/>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" ht="30" hidden="1">
       <c r="A174" s="30" t="s">
         <v>194</v>
       </c>
@@ -7949,7 +7951,7 @@
       </c>
       <c r="I174" s="32"/>
     </row>
-    <row r="175" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="30" hidden="1">
       <c r="A175" s="30" t="s">
         <v>195</v>
       </c>
@@ -7974,7 +7976,7 @@
       </c>
       <c r="I175" s="32"/>
     </row>
-    <row r="176" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="105" hidden="1">
       <c r="A176" s="30" t="s">
         <v>196</v>
       </c>
@@ -7999,7 +8001,7 @@
       </c>
       <c r="I176" s="32"/>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1">
       <c r="A177" s="30" t="s">
         <v>197</v>
       </c>
@@ -8024,7 +8026,7 @@
       </c>
       <c r="I177" s="32"/>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" ht="30" hidden="1">
       <c r="A178" s="30" t="s">
         <v>198</v>
       </c>
@@ -8049,7 +8051,7 @@
       </c>
       <c r="I178" s="32"/>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1">
       <c r="A179" s="30" t="s">
         <v>199</v>
       </c>
@@ -8074,7 +8076,7 @@
       </c>
       <c r="I179" s="32"/>
     </row>
-    <row r="180" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="30" hidden="1">
       <c r="A180" s="30" t="s">
         <v>200</v>
       </c>
@@ -8099,7 +8101,7 @@
       </c>
       <c r="I180" s="32"/>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1">
       <c r="A181" s="30" t="s">
         <v>201</v>
       </c>
@@ -8124,7 +8126,7 @@
       </c>
       <c r="I181" s="32"/>
     </row>
-    <row r="182" spans="1:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" ht="195" hidden="1">
       <c r="A182" s="30" t="s">
         <v>202</v>
       </c>
@@ -8149,7 +8151,7 @@
       </c>
       <c r="I182" s="32"/>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1">
       <c r="A183" s="30" t="s">
         <v>203</v>
       </c>
@@ -8174,7 +8176,7 @@
       </c>
       <c r="I183" s="32"/>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1">
       <c r="A184" s="30" t="s">
         <v>204</v>
       </c>
@@ -8199,7 +8201,7 @@
       </c>
       <c r="I184" s="32"/>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1">
       <c r="A185" s="30" t="s">
         <v>205</v>
       </c>
@@ -8224,7 +8226,7 @@
       </c>
       <c r="I185" s="32"/>
     </row>
-    <row r="186" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" ht="30" hidden="1">
       <c r="A186" s="30" t="s">
         <v>206</v>
       </c>
@@ -8249,7 +8251,7 @@
       </c>
       <c r="I186" s="32"/>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" ht="30" hidden="1">
       <c r="A187" s="30" t="s">
         <v>207</v>
       </c>
@@ -8274,7 +8276,7 @@
       </c>
       <c r="I187" s="32"/>
     </row>
-    <row r="188" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="30" hidden="1">
       <c r="A188" s="30" t="s">
         <v>208</v>
       </c>
@@ -8299,7 +8301,7 @@
       </c>
       <c r="I188" s="32"/>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1">
       <c r="A189" s="30" t="s">
         <v>209</v>
       </c>
@@ -8324,7 +8326,7 @@
       </c>
       <c r="I189" s="32"/>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1">
       <c r="A190" s="30" t="s">
         <v>210</v>
       </c>
@@ -8349,7 +8351,7 @@
       </c>
       <c r="I190" s="32"/>
     </row>
-    <row r="191" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="30" hidden="1">
       <c r="A191" s="30" t="s">
         <v>211</v>
       </c>
@@ -8374,7 +8376,7 @@
       </c>
       <c r="I191" s="32"/>
     </row>
-    <row r="192" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="75" hidden="1">
       <c r="A192" s="30" t="s">
         <v>212</v>
       </c>
@@ -8399,7 +8401,7 @@
       </c>
       <c r="I192" s="32"/>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" ht="30" hidden="1">
       <c r="A193" s="30" t="s">
         <v>213</v>
       </c>
@@ -8424,7 +8426,7 @@
       </c>
       <c r="I193" s="32"/>
     </row>
-    <row r="194" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="45" hidden="1">
       <c r="A194" s="30" t="s">
         <v>214</v>
       </c>
@@ -8449,7 +8451,7 @@
       </c>
       <c r="I194" s="32"/>
     </row>
-    <row r="195" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="60" hidden="1">
       <c r="A195" s="30" t="s">
         <v>215</v>
       </c>
@@ -8474,7 +8476,7 @@
       </c>
       <c r="I195" s="32"/>
     </row>
-    <row r="196" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="45" hidden="1">
       <c r="A196" s="30" t="s">
         <v>216</v>
       </c>
@@ -8499,7 +8501,7 @@
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="30" hidden="1">
       <c r="A197" s="30" t="s">
         <v>217</v>
       </c>
@@ -8524,7 +8526,7 @@
       </c>
       <c r="I197" s="32"/>
     </row>
-    <row r="198" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" ht="30" hidden="1">
       <c r="A198" s="30" t="s">
         <v>218</v>
       </c>
@@ -8549,7 +8551,7 @@
       </c>
       <c r="I198" s="32"/>
     </row>
-    <row r="199" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" ht="45" hidden="1">
       <c r="A199" s="30" t="s">
         <v>219</v>
       </c>
@@ -8574,7 +8576,7 @@
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="75" hidden="1">
       <c r="A200" s="30" t="s">
         <v>220</v>
       </c>
@@ -8599,7 +8601,7 @@
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="90" hidden="1">
       <c r="A201" s="30" t="s">
         <v>221</v>
       </c>
@@ -8624,7 +8626,7 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1">
       <c r="A202" s="30" t="s">
         <v>222</v>
       </c>
@@ -8649,7 +8651,7 @@
       </c>
       <c r="I202" s="32"/>
     </row>
-    <row r="203" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" ht="30" hidden="1">
       <c r="A203" s="30" t="s">
         <v>223</v>
       </c>
@@ -8674,7 +8676,7 @@
       </c>
       <c r="I203" s="32"/>
     </row>
-    <row r="204" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" ht="45" hidden="1">
       <c r="A204" s="30" t="s">
         <v>224</v>
       </c>
@@ -8699,7 +8701,7 @@
       </c>
       <c r="I204" s="32"/>
     </row>
-    <row r="205" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" ht="60" hidden="1">
       <c r="A205" s="30" t="s">
         <v>225</v>
       </c>
@@ -8724,7 +8726,7 @@
       </c>
       <c r="I205" s="32"/>
     </row>
-    <row r="206" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="30" hidden="1">
       <c r="A206" s="30" t="s">
         <v>226</v>
       </c>
@@ -8749,7 +8751,7 @@
       </c>
       <c r="I206" s="32"/>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1">
       <c r="A207" s="30" t="s">
         <v>227</v>
       </c>
@@ -8774,7 +8776,7 @@
       </c>
       <c r="I207" s="32"/>
     </row>
-    <row r="208" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" ht="30" hidden="1">
       <c r="A208" s="30" t="s">
         <v>228</v>
       </c>
@@ -8799,7 +8801,7 @@
       </c>
       <c r="I208" s="32"/>
     </row>
-    <row r="209" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="60" hidden="1">
       <c r="A209" s="30" t="s">
         <v>229</v>
       </c>
@@ -8824,7 +8826,7 @@
       </c>
       <c r="I209" s="32"/>
     </row>
-    <row r="210" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="60" hidden="1">
       <c r="A210" s="30" t="s">
         <v>230</v>
       </c>
@@ -8849,7 +8851,7 @@
       </c>
       <c r="I210" s="32"/>
     </row>
-    <row r="211" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="30" hidden="1">
       <c r="A211" s="30" t="s">
         <v>231</v>
       </c>
@@ -8874,7 +8876,7 @@
       </c>
       <c r="I211" s="32"/>
     </row>
-    <row r="212" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="30" hidden="1">
       <c r="A212" s="30" t="s">
         <v>232</v>
       </c>
@@ -8899,7 +8901,7 @@
       </c>
       <c r="I212" s="32"/>
     </row>
-    <row r="213" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="60" hidden="1">
       <c r="A213" s="22" t="s">
         <v>233</v>
       </c>
@@ -8907,7 +8909,7 @@
         <v>33</v>
       </c>
       <c r="C213" s="20" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D213" s="30"/>
       <c r="E213" s="30" t="s">
@@ -8924,7 +8926,7 @@
       </c>
       <c r="I213" s="32"/>
     </row>
-    <row r="214" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="75" hidden="1">
       <c r="A214" s="30" t="s">
         <v>234</v>
       </c>
@@ -8949,7 +8951,7 @@
       </c>
       <c r="I214" s="32"/>
     </row>
-    <row r="215" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="45" hidden="1">
       <c r="A215" s="30" t="s">
         <v>235</v>
       </c>
@@ -8974,7 +8976,7 @@
       </c>
       <c r="I215" s="32"/>
     </row>
-    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="30" hidden="1">
       <c r="A216" s="30" t="s">
         <v>236</v>
       </c>
@@ -8999,7 +9001,7 @@
       </c>
       <c r="I216" s="32"/>
     </row>
-    <row r="217" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="45" hidden="1">
       <c r="A217" s="22" t="s">
         <v>237</v>
       </c>
@@ -9026,7 +9028,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1">
       <c r="A218" s="30" t="s">
         <v>238</v>
       </c>
@@ -9051,7 +9053,7 @@
       </c>
       <c r="I218" s="32"/>
     </row>
-    <row r="219" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="30" hidden="1">
       <c r="A219" s="30" t="s">
         <v>239</v>
       </c>
@@ -9076,7 +9078,7 @@
       </c>
       <c r="I219" s="32"/>
     </row>
-    <row r="220" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="30" hidden="1">
       <c r="A220" s="30" t="s">
         <v>240</v>
       </c>
@@ -9101,7 +9103,7 @@
       </c>
       <c r="I220" s="32"/>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="30" hidden="1">
       <c r="A221" s="30" t="s">
         <v>241</v>
       </c>
@@ -9126,7 +9128,7 @@
       </c>
       <c r="I221" s="32"/>
     </row>
-    <row r="222" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="30" hidden="1">
       <c r="A222" s="30" t="s">
         <v>242</v>
       </c>
@@ -9151,7 +9153,7 @@
       </c>
       <c r="I222" s="32"/>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="30" hidden="1">
       <c r="A223" s="30" t="s">
         <v>243</v>
       </c>
@@ -9176,7 +9178,7 @@
       </c>
       <c r="I223" s="32"/>
     </row>
-    <row r="224" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="30" hidden="1">
       <c r="A224" s="30" t="s">
         <v>244</v>
       </c>
@@ -9201,7 +9203,7 @@
       </c>
       <c r="I224" s="32"/>
     </row>
-    <row r="225" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="195" hidden="1">
       <c r="A225" s="30" t="s">
         <v>245</v>
       </c>
@@ -9226,7 +9228,7 @@
       </c>
       <c r="I225" s="32"/>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1">
       <c r="A226" s="30" t="s">
         <v>246</v>
       </c>
@@ -9251,7 +9253,7 @@
       </c>
       <c r="I226" s="32"/>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1">
       <c r="A227" s="30" t="s">
         <v>247</v>
       </c>
@@ -9276,7 +9278,7 @@
       </c>
       <c r="I227" s="32"/>
     </row>
-    <row r="228" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="30" hidden="1">
       <c r="A228" s="30" t="s">
         <v>248</v>
       </c>
@@ -9301,7 +9303,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="30" hidden="1">
       <c r="A229" s="30" t="s">
         <v>249</v>
       </c>
@@ -9326,7 +9328,7 @@
       </c>
       <c r="I229" s="32"/>
     </row>
-    <row r="230" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="30" hidden="1">
       <c r="A230" s="30" t="s">
         <v>250</v>
       </c>
@@ -9351,7 +9353,7 @@
       </c>
       <c r="I230" s="32"/>
     </row>
-    <row r="231" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="45" hidden="1">
       <c r="A231" s="30" t="s">
         <v>251</v>
       </c>
@@ -9376,7 +9378,7 @@
       </c>
       <c r="I231" s="32"/>
     </row>
-    <row r="232" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="45" hidden="1">
       <c r="A232" s="30" t="s">
         <v>252</v>
       </c>
@@ -9401,7 +9403,7 @@
       </c>
       <c r="I232" s="32"/>
     </row>
-    <row r="233" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="30" hidden="1">
       <c r="A233" s="30" t="s">
         <v>253</v>
       </c>
@@ -9426,7 +9428,7 @@
       </c>
       <c r="I233" s="32"/>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1">
       <c r="A234" s="30" t="s">
         <v>254</v>
       </c>
@@ -9451,7 +9453,7 @@
       </c>
       <c r="I234" s="32"/>
     </row>
-    <row r="235" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="30" hidden="1">
       <c r="A235" s="30" t="s">
         <v>255</v>
       </c>
@@ -9476,7 +9478,7 @@
       </c>
       <c r="I235" s="32"/>
     </row>
-    <row r="236" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="30" hidden="1">
       <c r="A236" s="30" t="s">
         <v>256</v>
       </c>
@@ -9501,7 +9503,7 @@
       </c>
       <c r="I236" s="32"/>
     </row>
-    <row r="237" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="165" hidden="1">
       <c r="A237" s="30" t="s">
         <v>257</v>
       </c>
@@ -9526,7 +9528,7 @@
       </c>
       <c r="I237" s="32"/>
     </row>
-    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1">
       <c r="A238" s="30" t="s">
         <v>258</v>
       </c>
@@ -9551,7 +9553,7 @@
       </c>
       <c r="I238" s="32"/>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="30" hidden="1">
       <c r="A239" s="30" t="s">
         <v>259</v>
       </c>
@@ -9576,7 +9578,7 @@
       </c>
       <c r="I239" s="32"/>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="30" hidden="1">
       <c r="A240" s="30" t="s">
         <v>260</v>
       </c>
@@ -9601,7 +9603,7 @@
       </c>
       <c r="I240" s="32"/>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="30" hidden="1">
       <c r="A241" s="30" t="s">
         <v>261</v>
       </c>
@@ -9626,7 +9628,7 @@
       </c>
       <c r="I241" s="32"/>
     </row>
-    <row r="242" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="30" hidden="1">
       <c r="A242" s="30" t="s">
         <v>262</v>
       </c>
@@ -9651,7 +9653,7 @@
       </c>
       <c r="I242" s="32"/>
     </row>
-    <row r="243" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" ht="30">
       <c r="A243" s="30" t="s">
         <v>263</v>
       </c>
@@ -9676,7 +9678,7 @@
       </c>
       <c r="I243" s="32"/>
     </row>
-    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="30">
       <c r="A244" s="30" t="s">
         <v>264</v>
       </c>
@@ -9701,7 +9703,7 @@
       </c>
       <c r="I244" s="32"/>
     </row>
-    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="30">
       <c r="A245" s="30" t="s">
         <v>265</v>
       </c>
@@ -9726,7 +9728,7 @@
       </c>
       <c r="I245" s="32"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="30">
       <c r="A246" s="30" t="s">
         <v>266</v>
       </c>
@@ -9751,7 +9753,7 @@
       </c>
       <c r="I246" s="32"/>
     </row>
-    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="30">
       <c r="A247" s="30" t="s">
         <v>267</v>
       </c>
@@ -9776,7 +9778,7 @@
       </c>
       <c r="I247" s="32"/>
     </row>
-    <row r="248" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" ht="75">
       <c r="A248" s="30" t="s">
         <v>268</v>
       </c>
@@ -9801,7 +9803,7 @@
       </c>
       <c r="I248" s="32"/>
     </row>
-    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" ht="30">
       <c r="A249" s="30" t="s">
         <v>269</v>
       </c>
@@ -9826,7 +9828,7 @@
       </c>
       <c r="I249" s="32"/>
     </row>
-    <row r="250" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" ht="45">
       <c r="A250" s="30" t="s">
         <v>270</v>
       </c>
@@ -9851,7 +9853,7 @@
       </c>
       <c r="I250" s="32"/>
     </row>
-    <row r="251" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" ht="30">
       <c r="A251" s="30" t="s">
         <v>271</v>
       </c>
@@ -9876,7 +9878,7 @@
       </c>
       <c r="I251" s="32"/>
     </row>
-    <row r="252" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" ht="75">
       <c r="A252" s="22" t="s">
         <v>272</v>
       </c>
@@ -9901,15 +9903,15 @@
       </c>
       <c r="I252" s="32"/>
     </row>
-    <row r="253" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" ht="60">
       <c r="A253" s="22" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B253" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C253" s="20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D253" s="30"/>
       <c r="E253" s="30" t="s">
@@ -9926,15 +9928,15 @@
       </c>
       <c r="I253" s="32"/>
     </row>
-    <row r="254" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" ht="75">
       <c r="A254" s="22" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B254" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C254" s="20" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D254" s="34"/>
       <c r="E254" s="34" t="s">
@@ -9951,15 +9953,15 @@
       </c>
       <c r="I254" s="35"/>
     </row>
-    <row r="255" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" ht="75">
       <c r="A255" s="22" t="s">
+        <v>686</v>
+      </c>
+      <c r="B255" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="B255" s="24" t="s">
-        <v>688</v>
-      </c>
       <c r="C255" s="20" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D255" s="22"/>
       <c r="E255" s="22" t="s">
@@ -9976,15 +9978,15 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" ht="75">
       <c r="A256" s="22" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B256" s="31" t="s">
         <v>345</v>
       </c>
       <c r="C256" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D256" s="30"/>
       <c r="E256" s="30" t="s">
@@ -10001,7 +10003,7 @@
       </c>
       <c r="I256" s="32"/>
     </row>
-    <row r="257" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="60">
       <c r="A257" s="30" t="s">
         <v>273</v>
       </c>
@@ -10009,7 +10011,7 @@
         <v>345</v>
       </c>
       <c r="C257" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D257" s="30"/>
       <c r="E257" s="30" t="s">
@@ -10026,7 +10028,7 @@
       </c>
       <c r="I257" s="32"/>
     </row>
-    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="30" t="s">
         <v>274</v>
       </c>
@@ -10051,7 +10053,7 @@
       </c>
       <c r="I258" s="32"/>
     </row>
-    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" ht="30">
       <c r="A259" s="30" t="s">
         <v>275</v>
       </c>
@@ -10076,7 +10078,7 @@
       </c>
       <c r="I259" s="32"/>
     </row>
-    <row r="260" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="30">
       <c r="A260" s="30" t="s">
         <v>276</v>
       </c>
@@ -10101,7 +10103,7 @@
       </c>
       <c r="I260" s="32"/>
     </row>
-    <row r="261" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" ht="60">
       <c r="A261" s="22" t="s">
         <v>277</v>
       </c>
@@ -10128,7 +10130,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" ht="60">
       <c r="A262" s="30" t="s">
         <v>278</v>
       </c>
@@ -10153,7 +10155,7 @@
       </c>
       <c r="I262" s="32"/>
     </row>
-    <row r="263" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" ht="120">
       <c r="A263" s="22" t="s">
         <v>279</v>
       </c>
@@ -10161,7 +10163,7 @@
         <v>345</v>
       </c>
       <c r="C263" s="20" t="s">
-        <v>669</v>
+        <v>690</v>
       </c>
       <c r="D263" s="30"/>
       <c r="E263" s="30" t="s">
@@ -10177,10 +10179,10 @@
         <v>17</v>
       </c>
       <c r="I263" s="20" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="264" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" ht="30">
       <c r="A264" s="30" t="s">
         <v>280</v>
       </c>
@@ -10207,7 +10209,7 @@
       </c>
       <c r="I264" s="32"/>
     </row>
-    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" ht="30">
       <c r="A265" s="30" t="s">
         <v>281</v>
       </c>
@@ -10234,7 +10236,7 @@
       </c>
       <c r="I265" s="32"/>
     </row>
-    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" ht="30">
       <c r="A266" s="30" t="s">
         <v>282</v>
       </c>
@@ -10261,7 +10263,7 @@
       </c>
       <c r="I266" s="32"/>
     </row>
-    <row r="267" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" ht="75">
       <c r="A267" s="30" t="s">
         <v>283</v>
       </c>
@@ -10288,7 +10290,7 @@
       </c>
       <c r="I267" s="32"/>
     </row>
-    <row r="268" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" ht="60">
       <c r="A268" s="30" t="s">
         <v>284</v>
       </c>
@@ -10315,7 +10317,7 @@
       </c>
       <c r="I268" s="32"/>
     </row>
-    <row r="269" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" ht="60">
       <c r="A269" s="30" t="s">
         <v>285</v>
       </c>
@@ -10342,7 +10344,7 @@
       </c>
       <c r="I269" s="32"/>
     </row>
-    <row r="270" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" ht="30" hidden="1">
       <c r="A270" s="30" t="s">
         <v>286</v>
       </c>
@@ -10367,7 +10369,7 @@
       </c>
       <c r="I270" s="32"/>
     </row>
-    <row r="271" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" ht="30" hidden="1">
       <c r="A271" s="30" t="s">
         <v>287</v>
       </c>
@@ -10392,7 +10394,7 @@
       </c>
       <c r="I271" s="32"/>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" ht="30" hidden="1">
       <c r="A272" s="30" t="s">
         <v>288</v>
       </c>
@@ -10417,7 +10419,7 @@
       </c>
       <c r="I272" s="32"/>
     </row>
-    <row r="273" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" ht="30" hidden="1">
       <c r="A273" s="30" t="s">
         <v>289</v>
       </c>
@@ -10442,7 +10444,7 @@
       </c>
       <c r="I273" s="32"/>
     </row>
-    <row r="274" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" ht="30" hidden="1">
       <c r="A274" s="30" t="s">
         <v>290</v>
       </c>
@@ -10467,7 +10469,7 @@
       </c>
       <c r="I274" s="32"/>
     </row>
-    <row r="275" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" ht="30" hidden="1">
       <c r="A275" s="30" t="s">
         <v>291</v>
       </c>
@@ -10492,7 +10494,7 @@
       </c>
       <c r="I275" s="32"/>
     </row>
-    <row r="276" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" ht="150" hidden="1">
       <c r="A276" s="30" t="s">
         <v>292</v>
       </c>
@@ -10517,7 +10519,7 @@
       </c>
       <c r="I276" s="32"/>
     </row>
-    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" hidden="1">
       <c r="A277" s="30" t="s">
         <v>293</v>
       </c>
@@ -10542,7 +10544,7 @@
       </c>
       <c r="I277" s="32"/>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" hidden="1">
       <c r="A278" s="30" t="s">
         <v>294</v>
       </c>
@@ -10567,7 +10569,7 @@
       </c>
       <c r="I278" s="32"/>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" hidden="1">
       <c r="A279" s="30" t="s">
         <v>295</v>
       </c>
@@ -10592,7 +10594,7 @@
       </c>
       <c r="I279" s="32"/>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" ht="30" hidden="1">
       <c r="A280" s="30" t="s">
         <v>296</v>
       </c>
@@ -10617,7 +10619,7 @@
       </c>
       <c r="I280" s="32"/>
     </row>
-    <row r="281" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" ht="30" hidden="1">
       <c r="A281" s="30" t="s">
         <v>297</v>
       </c>
@@ -10642,7 +10644,7 @@
       </c>
       <c r="I281" s="32"/>
     </row>
-    <row r="282" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" ht="30" hidden="1">
       <c r="A282" s="30" t="s">
         <v>298</v>
       </c>
@@ -10667,7 +10669,7 @@
       </c>
       <c r="I282" s="32"/>
     </row>
-    <row r="283" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" ht="165" hidden="1">
       <c r="A283" s="30" t="s">
         <v>299</v>
       </c>
@@ -10692,7 +10694,7 @@
       </c>
       <c r="I283" s="32"/>
     </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" ht="30" hidden="1">
       <c r="A284" s="30" t="s">
         <v>300</v>
       </c>
@@ -10717,7 +10719,7 @@
       </c>
       <c r="I284" s="32"/>
     </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" ht="30" hidden="1">
       <c r="A285" s="30" t="s">
         <v>301</v>
       </c>
@@ -10742,7 +10744,7 @@
       </c>
       <c r="I285" s="32"/>
     </row>
-    <row r="286" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" ht="30" hidden="1">
       <c r="A286" s="30" t="s">
         <v>302</v>
       </c>
@@ -10767,7 +10769,7 @@
       </c>
       <c r="I286" s="32"/>
     </row>
-    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" ht="30" hidden="1">
       <c r="A287" s="30" t="s">
         <v>303</v>
       </c>
@@ -10792,7 +10794,7 @@
       </c>
       <c r="I287" s="32"/>
     </row>
-    <row r="288" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" ht="30" hidden="1">
       <c r="A288" s="30" t="s">
         <v>304</v>
       </c>
@@ -10817,7 +10819,7 @@
       </c>
       <c r="I288" s="32"/>
     </row>
-    <row r="289" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" ht="45" hidden="1">
       <c r="A289" s="30" t="s">
         <v>305</v>
       </c>
@@ -10846,7 +10848,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="290" spans="1:9" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" s="33" customFormat="1" ht="45" hidden="1">
       <c r="A290" s="22" t="s">
         <v>306</v>
       </c>
@@ -10857,7 +10859,7 @@
         <v>599</v>
       </c>
       <c r="D290" s="22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E290" s="30" t="s">
         <v>22</v>
@@ -10875,7 +10877,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="291" spans="1:9" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" s="33" customFormat="1" ht="45" hidden="1">
       <c r="A291" s="30" t="s">
         <v>307</v>
       </c>
@@ -10886,7 +10888,7 @@
         <v>600</v>
       </c>
       <c r="D291" s="22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E291" s="30" t="s">
         <v>22</v>
@@ -10904,7 +10906,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" ht="60" hidden="1">
       <c r="A292" s="30" t="s">
         <v>308</v>
       </c>
@@ -10912,7 +10914,7 @@
         <v>350</v>
       </c>
       <c r="C292" s="20" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D292" s="22" t="s">
         <v>625</v>
@@ -10933,7 +10935,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" ht="60" hidden="1">
       <c r="A293" s="30" t="s">
         <v>309</v>
       </c>
@@ -10941,7 +10943,7 @@
         <v>350</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D293" s="30" t="s">
         <v>625</v>
@@ -10962,7 +10964,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="294" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" ht="45" hidden="1">
       <c r="A294" s="30" t="s">
         <v>310</v>
       </c>
@@ -10991,7 +10993,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="295" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" ht="45" hidden="1">
       <c r="A295" s="30" t="s">
         <v>311</v>
       </c>
@@ -11020,7 +11022,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="296" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" ht="45" hidden="1">
       <c r="A296" s="30" t="s">
         <v>312</v>
       </c>
@@ -11049,7 +11051,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="297" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" ht="30" hidden="1">
       <c r="A297" s="22" t="s">
         <v>649</v>
       </c>
@@ -11076,7 +11078,7 @@
       </c>
       <c r="I297" s="32"/>
     </row>
-    <row r="298" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" ht="30" hidden="1">
       <c r="A298" s="22" t="s">
         <v>653</v>
       </c>
@@ -11103,7 +11105,7 @@
       </c>
       <c r="I298" s="32"/>
     </row>
-    <row r="299" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" ht="45" hidden="1">
       <c r="A299" s="30" t="s">
         <v>313</v>
       </c>
@@ -11111,7 +11113,7 @@
         <v>350</v>
       </c>
       <c r="C299" s="20" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D299" s="22" t="s">
         <v>627</v>
@@ -11132,7 +11134,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" ht="45" hidden="1">
       <c r="A300" s="30" t="s">
         <v>314</v>
       </c>
@@ -11140,7 +11142,7 @@
         <v>350</v>
       </c>
       <c r="C300" s="20" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D300" s="30" t="s">
         <v>627</v>
@@ -11161,7 +11163,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="301" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" ht="45" hidden="1">
       <c r="A301" s="22" t="s">
         <v>656</v>
       </c>
@@ -11188,7 +11190,7 @@
       </c>
       <c r="I301" s="32"/>
     </row>
-    <row r="302" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" ht="45" hidden="1">
       <c r="A302" s="22" t="s">
         <v>658</v>
       </c>
@@ -11196,7 +11198,7 @@
         <v>350</v>
       </c>
       <c r="C302" s="20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D302" s="22" t="s">
         <v>657</v>
@@ -11217,7 +11219,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="303" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" ht="60" hidden="1">
       <c r="A303" s="22" t="s">
         <v>666</v>
       </c>
@@ -11246,7 +11248,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="304" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" ht="45" hidden="1">
       <c r="A304" s="22" t="s">
         <v>315</v>
       </c>
@@ -11271,7 +11273,7 @@
       </c>
       <c r="I304" s="32"/>
     </row>
-    <row r="305" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" ht="30" hidden="1">
       <c r="A305" s="30" t="s">
         <v>316</v>
       </c>
@@ -11296,11 +11298,11 @@
       </c>
       <c r="I305" s="32"/>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9">
       <c r="A306" s="3"/>
       <c r="B306" s="10"/>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9">
       <c r="A307" s="3"/>
       <c r="B307" s="10"/>
     </row>

</xml_diff>